<commit_message>
📊 Horarios actualizados Línea 141 - 358
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:03:48</t>
+          <t>Última actualización: 01:50:13</t>
         </is>
       </c>
     </row>
@@ -487,21 +487,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:03:48</t>
+          <t>01:50:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>01:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,21 +512,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:03:48</t>
+          <t>01:50:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>03:12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:03:48</t>
+          <t>01:50:13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,14 +588,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:03:48</t>
+          <t>Última actualización: 01:50:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 1</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:03:48</t>
+          <t>01:50:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:12</t>
+          <t>03:12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -643,34 +643,9 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>01:03:48</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>02:58</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>115</v>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -705,7 +680,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:03:48</t>
+          <t>Última actualización: 01:50:13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 359
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:50:13</t>
+          <t>Última actualización: 02:15:29</t>
         </is>
       </c>
     </row>
@@ -487,21 +487,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:50:13</t>
+          <t>02:15:29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,21 +512,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>01:50:13</t>
+          <t>02:15:29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:12</t>
+          <t>03:56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>01:50:13</t>
+          <t>02:15:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:50:13</t>
+          <t>Última actualización: 02:15:29</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>01:50:13</t>
+          <t>02:15:29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:12</t>
+          <t>02:58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 01:50:13</t>
+          <t>Última actualización: 02:15:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 360
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:15:29</t>
+          <t>Última actualización: 02:43:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -487,12 +487,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:15:29</t>
+          <t>02:43:45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:43</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,12 +512,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:15:29</t>
+          <t>02:43:45</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:56</t>
+          <t>03:54</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:15:29</t>
+          <t>02:43:45</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -551,9 +551,34 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>78</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>02:43:45</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04:29</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>106</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -570,7 +595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,14 +613,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:15:29</t>
+          <t>Última actualización: 02:43:45</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 2</t>
         </is>
       </c>
     </row>
@@ -629,12 +654,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:15:29</t>
+          <t>02:43:45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:58</t>
+          <t>02:43</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -643,9 +668,34 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>02:43:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:29</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>106</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -680,7 +730,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:15:29</t>
+          <t>Última actualización: 02:43:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 361
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:43:45</t>
+          <t>Última actualización: 02:56:21</t>
         </is>
       </c>
     </row>
@@ -487,21 +487,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:43:45</t>
+          <t>02:56:21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:43</t>
+          <t>03:55</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,21 +512,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:43:45</t>
+          <t>02:56:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03:54</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:43:45</t>
+          <t>02:56:21</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:31</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,21 +562,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:43:45</t>
+          <t>02:56:21</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:29</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,14 +613,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:43:45</t>
+          <t>Última actualización: 02:56:21</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 1</t>
         </is>
       </c>
     </row>
@@ -654,12 +654,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:43:45</t>
+          <t>02:56:21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>02:43</t>
+          <t>04:31</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,34 +668,9 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>02:43:45</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>04:29</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -730,7 +705,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:43:45</t>
+          <t>Última actualización: 02:56:21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 362
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:56:21</t>
+          <t>Última actualización: 03:24:15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -487,12 +487,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:56:21</t>
+          <t>03:24:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:55</t>
+          <t>03:48</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>02:56:21</t>
+          <t>03:24:15</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,12 +537,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>02:56:21</t>
+          <t>03:24:15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:31</t>
+          <t>04:32</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>02:56:21</t>
+          <t>03:24:15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -576,9 +576,59 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>03:24:15</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:16</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>112</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>03:24:15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>118</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -613,7 +663,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:56:21</t>
+          <t>Última actualización: 03:24:15</t>
         </is>
       </c>
     </row>
@@ -654,12 +704,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>02:56:21</t>
+          <t>03:24:15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:31</t>
+          <t>04:32</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,7 +718,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -705,7 +755,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 02:56:21</t>
+          <t>Última actualización: 03:24:15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 363
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:24:15</t>
+          <t>Última actualización: 03:55:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -487,21 +487,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03:48</t>
+          <t>04:01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -512,21 +512,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>04:01</t>
+          <t>04:34</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:32</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -562,21 +562,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -587,21 +587,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,23 +612,48 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>03:55:13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>111</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -640,6 +665,123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LÍNEA 141 - LP1912-215 - 15/01/2026</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Última actualización: 03:55:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Total filas: 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Linea</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Parada</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>03:55:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>04:34</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>39</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03:55:13</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -656,14 +798,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - LP1912-215 - 15/01/2026</t>
+          <t>LÍNEA 141 - 6203-6173 - 15/01/2026</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:24:15</t>
+          <t>Última actualización: 03:55:13</t>
         </is>
       </c>
     </row>
@@ -704,65 +846,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03:24:15</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>04:32</t>
+          <t>05:44</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>LP1912</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LÍNEA 141 - 6203-6173 - 15/01/2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Última actualización: 03:24:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Total filas: 0</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 364
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:55:13</t>
+          <t>Última actualización: 04:18:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -537,21 +537,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03:55:13</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04:53</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -567,16 +567,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:53</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,21 +612,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03:55:13</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -642,18 +642,193 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>05:22</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>87</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>76</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>03:55:13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05:35</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>03:55:13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>05:46</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D15" t="n">
         <v>111</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>05:53</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>95</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>06:05</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>107</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>113</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>06:13</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>115</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -670,7 +845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -688,14 +863,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:55:13</t>
+          <t>Última actualización: 04:18:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 2</t>
+          <t>Total filas: 5</t>
         </is>
       </c>
     </row>
@@ -754,23 +929,98 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>27</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05:34</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>76</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>03:55:13</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>05:35</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>100</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>113</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -787,7 +1037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -805,14 +1055,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 03:55:13</t>
+          <t>Última actualización: 04:18:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 1</t>
+          <t>Total filas: 3</t>
         </is>
       </c>
     </row>
@@ -846,23 +1096,73 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05:43</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>85</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>03:55:13</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>05:44</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>109</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>06:08</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>110</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 365
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:18:52</t>
+          <t>Última actualización: 04:40:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -762,21 +762,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>04:40:48</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06:05</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -787,21 +787,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>04:40:48</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -817,18 +817,193 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>06:05</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>107</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>06:11</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>113</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>04:18:52</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>06:13</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>225_HARAS DEL SUR</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D21" t="n">
         <v>115</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>06:14</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>225_HARAS DEL SUR</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>94</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>06:21</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>101</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>06:27</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>107</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>109</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>06:31</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>111</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -863,7 +1038,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:18:52</t>
+          <t>Última actualización: 04:40:48</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1055,14 +1230,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:18:52</t>
+          <t>Última actualización: 04:40:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 3</t>
+          <t>Total filas: 4</t>
         </is>
       </c>
     </row>
@@ -1165,6 +1340,31 @@
       <c r="E8" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:32</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>112</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 366
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:40:48</t>
+          <t>Última actualización: 04:54:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -587,21 +587,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03:55:13</t>
+          <t>04:54:17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>05:16</t>
+          <t>04:54</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -612,21 +612,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05:21</t>
+          <t>05:16</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -637,12 +637,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03:55:13</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>05:22</t>
+          <t>05:21</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -662,21 +662,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>05:34</t>
+          <t>05:22</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -687,12 +687,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03:55:13</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>05:35</t>
+          <t>05:34</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>05:35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -737,21 +737,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>03:55:13</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>05:53</t>
+          <t>05:46</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -762,12 +762,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>04:40:48</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>05:54</t>
+          <t>05:53</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -792,16 +792,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06:04</t>
+          <t>05:54</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -812,12 +812,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>04:18:52</t>
+          <t>04:40:48</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06:05</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -842,16 +842,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06:11</t>
+          <t>06:05</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -867,16 +867,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06:13</t>
+          <t>06:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>225_HARAS DEL SUR</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -887,12 +887,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>04:40:48</t>
+          <t>04:18:52</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06:14</t>
+          <t>06:13</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -917,16 +917,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06:21</t>
+          <t>06:14</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_HARAS DEL SUR</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -942,16 +942,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06:27</t>
+          <t>06:21</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -967,16 +967,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>06:29</t>
+          <t>06:27</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -992,18 +992,93 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>06:29</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>109</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04:40:48</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>06:31</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D27" t="n">
         <v>111</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04:54:17</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>06:44</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>110</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>04:54:17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>112</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1020,7 +1095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1038,14 +1113,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:40:48</t>
+          <t>Última actualización: 04:54:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 5</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1196,6 +1271,31 @@
         <v>113</v>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04:54:17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>112</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1212,7 +1312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,14 +1330,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:40:48</t>
+          <t>Última actualización: 04:54:17</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 4</t>
+          <t>Total filas: 6</t>
         </is>
       </c>
     </row>
@@ -1346,23 +1446,73 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>04:54:17</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>06:09</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>75</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>04:40:48</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>06:32</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>112</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>04:54:17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>06:33</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>99</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 367
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:54:17</t>
+          <t>Última actualización: 05:19:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -1079,6 +1079,131 @@
         <v>112</v>
       </c>
       <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>06:59</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>100</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>106</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>108</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>112</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>07:15</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>116</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1095,7 +1220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,14 +1238,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:54:17</t>
+          <t>Última actualización: 05:19:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1296,6 +1421,31 @@
         <v>112</v>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>112</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1312,7 +1462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1330,14 +1480,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 04:54:17</t>
+          <t>Última actualización: 05:19:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 6</t>
+          <t>Total filas: 7</t>
         </is>
       </c>
     </row>
@@ -1515,6 +1665,31 @@
       <c r="E11" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>101</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 368
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:19:24</t>
+          <t>Última actualización: 05:49:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -1012,21 +1012,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>04:40:48</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06:31</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1037,21 +1037,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>04:54:17</t>
+          <t>04:40:48</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06:44</t>
+          <t>06:31</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1067,16 +1067,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06:46</t>
+          <t>06:44</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1087,21 +1087,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>04:54:17</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06:59</t>
+          <t>06:46</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1112,21 +1112,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>06:47</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>06:59</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1162,21 +1162,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1187,23 +1187,323 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>76</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>05:19:24</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>07:05</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>106</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>07:07</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>108</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>07:11</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>112</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>05:19:24</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>07:15</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D38" t="n">
         <v>116</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>07:16</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>87</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>07:21</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>92</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>103</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>103</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>103</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>108</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>110</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>07:48</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>119</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1220,7 +1520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,14 +1538,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:19:24</t>
+          <t>Última actualización: 05:49:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1429,23 +1729,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:47</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>58</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>05:19:24</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>07:11</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>112</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1462,7 +1787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1480,14 +1805,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:19:24</t>
+          <t>Última actualización: 05:49:10</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 7</t>
+          <t>Total filas: 8</t>
         </is>
       </c>
     </row>
@@ -1688,6 +2013,31 @@
         <v>101</v>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>07:35</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>106</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 369
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:49:10</t>
+          <t>Última actualización: 06:14:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -1187,21 +1187,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>07:01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1242,16 +1242,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07:07</t>
+          <t>07:05</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1267,16 +1267,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>07:11</t>
+          <t>07:07</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1292,16 +1292,16 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>07:11</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1312,12 +1312,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>07:16</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1342,16 +1342,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:16</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1367,16 +1367,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,21 +1412,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1442,16 +1442,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1467,16 +1467,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1492,18 +1492,193 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>07:32</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>103</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07:37</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>108</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07:39</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>110</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07:47</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>93</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>05:49:10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>07:48</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D46" t="n">
+      <c r="D50" t="n">
         <v>119</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>97</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>106</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>118</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1520,7 +1695,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,14 +1713,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:49:10</t>
+          <t>Última actualización: 06:14:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -1771,6 +1946,31 @@
         <v>112</v>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>07:51</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>97</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1787,7 +1987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1805,14 +2005,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 05:49:10</t>
+          <t>Última actualización: 06:14:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 8</t>
+          <t>Total filas: 9</t>
         </is>
       </c>
     </row>
@@ -2040,6 +2240,31 @@
       <c r="E13" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08:07</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>113</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 370
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:14:19</t>
+          <t>Última actualización: 06:43:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 48</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -1362,21 +1362,21 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:17</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1417,16 +1417,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1437,12 +1437,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1497,7 +1497,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1517,16 +1517,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1542,16 +1542,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1562,21 +1562,21 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,12 +1587,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1642,16 +1642,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,23 +1662,198 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>69</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>06:14:19</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>106</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>08:03</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>80</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>08:12</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D56" t="n">
         <v>118</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>98</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>100</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>100</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>104</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1695,7 +1870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1713,14 +1888,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:14:19</t>
+          <t>Última actualización: 06:43:12</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -1971,6 +2146,56 @@
         <v>97</v>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>07:52</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>69</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2005,7 +2230,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:14:19</t>
+          <t>Última actualización: 06:43:12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 371
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:43:12</t>
+          <t>Última actualización: 06:57:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 58</t>
         </is>
       </c>
     </row>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:05</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1792,16 +1792,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1842,18 +1842,93 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>100</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>08:27</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
-      <c r="D60" t="n">
+      <c r="D61" t="n">
         <v>104</v>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>105</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>117</v>
+      </c>
+      <c r="E63" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1888,7 +1963,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:43:12</t>
+          <t>Última actualización: 06:57:11</t>
         </is>
       </c>
     </row>
@@ -2212,7 +2287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2230,14 +2305,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:43:12</t>
+          <t>Última actualización: 06:57:11</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 9</t>
+          <t>Total filas: 11</t>
         </is>
       </c>
     </row>
@@ -2490,6 +2565,56 @@
       <c r="E14" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>73</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>101</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 372
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:57:11</t>
+          <t>Última actualización: 07:19:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 58</t>
+          <t>Total filas: 70</t>
         </is>
       </c>
     </row>
@@ -1387,21 +1387,21 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>07:21</t>
+          <t>07:19</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1412,21 +1412,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07:23</t>
+          <t>07:21</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1442,16 +1442,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07:31</t>
+          <t>07:23</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1462,12 +1462,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,21 +1487,21 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07:32</t>
+          <t>07:31</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1542,16 +1542,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07:37</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1567,16 +1567,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07:39</t>
+          <t>07:32</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1587,21 +1587,21 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:34</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1612,21 +1612,21 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:36</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1637,21 +1637,21 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:37</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1662,21 +1662,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>07:39</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1692,16 +1692,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,21 +1712,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>08:05</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,21 +1762,21 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>07:52</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1837,21 +1837,21 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1867,16 +1867,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1892,16 +1892,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:05</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,23 +1912,323 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>51</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>06:14:19</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>08:12</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>08:21</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>98</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>08:22</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>63</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>100</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>08:23</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>06:43:12</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>08:27</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>104</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>06:57:11</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>08:42</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>105</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>84</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>08:54</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D63" t="n">
+      <c r="D72" t="n">
         <v>117</v>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>102</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>111</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>09:16</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>117</v>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -1945,7 +2245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1963,14 +2263,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:57:11</t>
+          <t>Última actualización: 07:19:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 12</t>
         </is>
       </c>
     </row>
@@ -2271,6 +2571,31 @@
         <v>100</v>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>102</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2287,7 +2612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2305,14 +2630,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 06:57:11</t>
+          <t>Última actualización: 07:19:37</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 11</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -2546,37 +2871,37 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08:07</t>
+          <t>07:38</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>08:07</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2585,7 +2910,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2596,25 +2921,125 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08:08</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>49</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>06:57:11</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08:10</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>73</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>08:35</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>76</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>08:38</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="D19" t="n">
         <v>101</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>109</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 373
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:19:37</t>
+          <t>Última actualización: 07:45:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 70</t>
+          <t>Total filas: 81</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1497,11 +1497,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1687,21 +1687,21 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:46</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1712,12 +1712,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>07:47</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1726,7 +1726,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1737,21 +1737,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07:51</t>
+          <t>07:48</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1762,12 +1762,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>07:51</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1776,7 +1776,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1787,21 +1787,21 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:52</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1812,21 +1812,21 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:55</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1842,16 +1842,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>07:59</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1862,12 +1862,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1876,7 +1876,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1887,21 +1887,21 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08:05</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,21 +1912,21 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>08:03</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:05</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1962,21 +1962,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2042,16 +2042,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2112,21 +2112,21 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2137,21 +2137,21 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,21 +2162,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,21 +2187,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2217,18 +2217,293 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>08:43</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>84</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>08:54</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>117</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>09:01</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>102</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>09:03</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>78</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>111</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>09:16</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D75" t="n">
+      <c r="D80" t="n">
         <v>117</v>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>96</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>97</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>98</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>107</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>108</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>116</v>
+      </c>
+      <c r="E86" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2245,7 +2520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2263,14 +2538,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:19:37</t>
+          <t>Última actualización: 07:45:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 12</t>
+          <t>Total filas: 13</t>
         </is>
       </c>
     </row>
@@ -2596,6 +2871,31 @@
         <v>102</v>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>116</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2612,7 +2912,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2630,14 +2930,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:19:37</t>
+          <t>Última actualización: 07:45:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 16</t>
         </is>
       </c>
     </row>
@@ -2946,12 +3246,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08:10</t>
+          <t>08:09</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2960,7 +3260,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2971,37 +3271,37 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:10</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3010,7 +3310,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3021,23 +3321,48 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>101</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>07:19:37</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>09:08</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>109</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 374
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:45:49</t>
+          <t>Última actualización: 07:58:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 81</t>
+          <t>Total filas: 90</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1987,21 +1987,21 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>08:12</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2012,21 +2012,21 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>08:13</t>
+          <t>08:12</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2037,21 +2037,21 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>08:21</t>
+          <t>08:13</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2062,21 +2062,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>08:22</t>
+          <t>08:21</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2087,21 +2087,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>08:23</t>
+          <t>08:22</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2142,16 +2142,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>08:27</t>
+          <t>08:23</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2162,21 +2162,21 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>08:31</t>
+          <t>08:27</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2187,21 +2187,21 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:31</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>105</v>
+        <v>46</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2212,21 +2212,21 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:33</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2237,21 +2237,21 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2262,21 +2262,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,21 +2287,21 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2317,16 +2317,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,17 +2337,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2392,16 +2392,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2492,18 +2492,243 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>09:21</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>96</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>09:22</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>97</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>98</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>09:23</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>85</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>09:32</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>107</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>108</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
           <t>09:41</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D86" t="n">
+      <c r="D92" t="n">
         <v>116</v>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>104</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>105</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>114</v>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2520,7 +2745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2538,14 +2763,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:45:49</t>
+          <t>Última actualización: 07:58:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 13</t>
+          <t>Total filas: 14</t>
         </is>
       </c>
     </row>
@@ -2896,6 +3121,31 @@
         <v>116</v>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>104</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2912,7 +3162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2930,14 +3180,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:45:49</t>
+          <t>Última actualización: 07:58:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 16</t>
+          <t>Total filas: 19</t>
         </is>
       </c>
     </row>
@@ -3296,37 +3546,37 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>08:35</t>
+          <t>08:11</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>08:38</t>
+          <t>08:35</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -3335,7 +3585,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -3346,23 +3596,98 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>06:57:11</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>08:38</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>101</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>08:40</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>42</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>07:19:37</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>09:08</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="D23" t="n">
         <v>109</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:09</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>71</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 375
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:58:19</t>
+          <t>Última actualización: 08:19:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 90</t>
+          <t>Total filas: 96</t>
         </is>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2272,11 +2272,11 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2337,21 +2337,21 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>117</v>
+        <v>24</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,21 +2362,21 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2417,16 +2417,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2592,16 +2592,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:25</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,23 +2712,173 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>108</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>116</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
           <t>07:58:19</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>104</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>105</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
         <is>
           <t>09:52</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D95" t="n">
+      <c r="D99" t="n">
         <v>114</v>
       </c>
-      <c r="E95" t="inlineStr">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>111</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>113</v>
+      </c>
+      <c r="E101" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2763,7 +2913,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:58:19</t>
+          <t>Última actualización: 08:19:34</t>
         </is>
       </c>
     </row>
@@ -3162,7 +3312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3180,14 +3330,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 07:58:19</t>
+          <t>Última actualización: 08:19:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 19</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -3646,50 +3796,100 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>07:19:37</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>109</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>07:58:19</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>09:09</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="D25" t="n">
         <v>71</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>104</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 376
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:19:34</t>
+          <t>Última actualización: 08:36:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 96</t>
+          <t>Total filas: 104</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2262,21 +2262,21 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>08:42</t>
+          <t>08:38</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,21 +2312,21 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:42</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2367,16 +2367,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:43</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2387,21 +2387,21 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:46</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:25</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2692,16 +2692,16 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2717,16 +2717,16 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2742,16 +2742,16 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2767,16 +2767,16 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:25</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,12 +2812,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2826,7 +2826,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,23 +2862,223 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
+          <t>07:45:49</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>09:41</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>116</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>104</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>105</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>114</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
           <t>08:19:33</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>111</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
         <is>
           <t>10:12</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D101" t="n">
+      <c r="D106" t="n">
         <v>113</v>
       </c>
-      <c r="E101" t="inlineStr">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>105</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>106</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>110</v>
+      </c>
+      <c r="E109" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -2895,7 +3095,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2913,14 +3113,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:19:34</t>
+          <t>Última actualización: 08:36:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 14</t>
+          <t>Total filas: 15</t>
         </is>
       </c>
     </row>
@@ -3296,6 +3496,31 @@
         <v>104</v>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>110</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3312,7 +3537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3330,14 +3555,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:19:34</t>
+          <t>Última actualización: 08:36:20</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 22</t>
         </is>
       </c>
     </row>
@@ -3871,23 +4096,48 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>34</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>08:19:33</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="D27" t="n">
         <v>104</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 377
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:36:20</t>
+          <t>Última actualización: 08:48:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 104</t>
+          <t>Total filas: 116</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2412,21 +2412,21 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>08:53</t>
+          <t>08:49</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,21 +2437,21 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>08:54</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2462,21 +2462,21 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:54</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,21 +2537,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,21 +2587,21 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2617,16 +2617,16 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2642,16 +2642,16 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2662,21 +2662,21 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2737,21 +2737,21 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:25</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2817,16 +2817,16 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2842,16 +2842,16 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2867,16 +2867,16 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2892,16 +2892,16 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:25</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,21 +2987,21 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3012,21 +3012,21 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,23 +3062,323 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>104</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>09:43</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>105</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>09:44</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>56</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>09:52</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>114</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>10:10</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>111</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>10:11</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>83</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>10:12</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>113</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
           <t>08:36:20</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>105</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>106</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
         <is>
           <t>10:26</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="C118" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D109" t="n">
+      <c r="D118" t="n">
         <v>110</v>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>99</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>114</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>10:44</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>116</v>
+      </c>
+      <c r="E121" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3095,7 +3395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3113,14 +3413,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:36:20</t>
+          <t>Última actualización: 08:48:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 15</t>
+          <t>Total filas: 17</t>
         </is>
       </c>
     </row>
@@ -3454,21 +3754,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3479,12 +3779,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3493,7 +3793,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -3504,23 +3804,73 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>07:58:19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>09:42</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>104</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>08:36:20</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>10:26</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>110</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>99</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3537,7 +3887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3555,14 +3905,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:36:20</t>
+          <t>Última actualización: 08:48:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 22</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -4046,37 +4396,37 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>08:53</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4085,7 +4435,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -4096,12 +4446,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:09</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4110,7 +4460,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4121,23 +4471,73 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>09:10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>34</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>25</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>08:19:33</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="D29" t="n">
         <v>104</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 378
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:09</t>
+          <t>Última actualización: 08:55:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 116</t>
+          <t>Total filas: 121</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2487,21 +2487,21 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>09:01</t>
+          <t>08:56</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2512,21 +2512,21 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>08:56</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2537,12 +2537,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>09:02</t>
+          <t>09:01</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2551,7 +2551,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2562,21 +2562,21 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2592,16 +2592,16 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>09:04</t>
+          <t>09:02</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2612,21 +2612,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>09:05</t>
+          <t>09:03</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2637,21 +2637,21 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:04</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2667,16 +2667,16 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:05</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2687,21 +2687,21 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>09:11</t>
+          <t>09:06</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2712,21 +2712,21 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2742,16 +2742,16 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,21 +2762,21 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>09:16</t>
+          <t>09:11</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,21 +2787,21 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>09:17</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,21 +2812,21 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>09:21</t>
+          <t>09:13</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2837,21 +2837,21 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>09:22</t>
+          <t>09:14</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2862,21 +2862,21 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:16</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2892,16 +2892,16 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>09:23</t>
+          <t>09:17</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2912,21 +2912,21 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>09:24</t>
+          <t>09:21</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2937,21 +2937,21 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>09:25</t>
+          <t>09:22</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2962,21 +2962,21 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>09:32</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2992,16 +2992,16 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>09:33</t>
+          <t>09:23</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3017,16 +3017,16 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:24</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3037,21 +3037,21 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:25</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3062,21 +3062,21 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:32</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3087,21 +3087,21 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:33</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3117,16 +3117,16 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,21 +3162,21 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3187,21 +3187,21 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,21 +3212,21 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:21</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,23 +3362,148 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>106</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>110</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
           <t>08:48:09</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>99</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>114</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>08:55:19</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>108</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
         <is>
           <t>10:44</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C126" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D121" t="n">
+      <c r="D126" t="n">
         <v>116</v>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E126" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3413,7 +3538,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:09</t>
+          <t>Última actualización: 08:55:19</t>
         </is>
       </c>
     </row>
@@ -3887,7 +4012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3905,14 +4030,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:48:09</t>
+          <t>Última actualización: 08:55:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -4421,37 +4546,37 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>09:08</t>
+          <t>08:55</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215D_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>09:09</t>
+          <t>09:08</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -4460,7 +4585,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -4471,12 +4596,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>09:10</t>
+          <t>09:09</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4485,7 +4610,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -4496,12 +4621,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:10</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4510,7 +4635,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -4521,23 +4646,73 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>09:13</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>25</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>08:19:33</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>10:03</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>104</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>08:55:19</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>119</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 379
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:55:19</t>
+          <t>Última actualización: 09:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 121</t>
+          <t>Total filas: 136</t>
         </is>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3112,12 +3112,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>09:35</t>
+          <t>09:34</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3126,7 +3126,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3137,21 +3137,21 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>09:41</t>
+          <t>09:35</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3162,12 +3162,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>09:42</t>
+          <t>09:41</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3176,7 +3176,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3192,16 +3192,16 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>09:43</t>
+          <t>09:42</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3212,12 +3212,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>09:43</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3226,7 +3226,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3237,21 +3237,21 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>09:52</t>
+          <t>09:44</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3262,21 +3262,21 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>10:10</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,21 +3287,21 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>10:11</t>
+          <t>09:52</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3312,21 +3312,21 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>10:12</t>
+          <t>09:58</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3337,21 +3337,21 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>10:21</t>
+          <t>10:03</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3362,21 +3362,21 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>10:22</t>
+          <t>10:04</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3387,21 +3387,21 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>10:26</t>
+          <t>10:10</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3417,16 +3417,16 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>10:27</t>
+          <t>10:11</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3437,21 +3437,21 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,21 +3462,21 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:55:19</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:12</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3487,23 +3487,398 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>10:20</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>55</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>10:21</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>105</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>106</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>10:22</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>57</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>10:23</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>58</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>08:36:20</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>10:26</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>110</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
           <t>08:48:09</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>10:27</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>99</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>10:41</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>76</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>10:42</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>114</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>08:55:19</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>10:43</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>108</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>08:48:09</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
         <is>
           <t>10:44</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
+      <c r="C136" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D126" t="n">
+      <c r="D136" t="n">
         <v>116</v>
       </c>
-      <c r="E126" t="inlineStr">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>88</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>96</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>105</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>114</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>11:20</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>115</v>
+      </c>
+      <c r="E141" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3520,7 +3895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3538,14 +3913,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:55:19</t>
+          <t>Última actualización: 09:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 17</t>
+          <t>Total filas: 18</t>
         </is>
       </c>
     </row>
@@ -3996,6 +4371,31 @@
         <v>99</v>
       </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>96</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4012,7 +4412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4030,14 +4430,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 08:55:19</t>
+          <t>Última actualización: 09:25:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -4671,12 +5071,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>10:02</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -4685,7 +5085,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>104</v>
+        <v>37</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -4696,25 +5096,100 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>08:19:33</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10:03</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>104</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>88</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>08:55:19</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>10:54</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D33" t="n">
         <v>119</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>11:13</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>108</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 380
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:25:56</t>
+          <t>Última actualización: 10:12:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 136</t>
+          <t>Total filas: 157</t>
         </is>
       </c>
     </row>
@@ -3662,21 +3662,21 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>10:41</t>
+          <t>10:33</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3687,21 +3687,21 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>10:42</t>
+          <t>10:34</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3712,21 +3712,21 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>08:55:19</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>10:43</t>
+          <t>10:35</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3737,21 +3737,21 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>10:44</t>
+          <t>10:41</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3762,21 +3762,21 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>10:53</t>
+          <t>10:42</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3787,21 +3787,21 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:55:19</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:43</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3812,21 +3812,21 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>10:44</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3837,21 +3837,21 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3867,18 +3867,543 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>88</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>10:53</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>41</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>10:56</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>44</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>96</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>50</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>11:03</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>51</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>11:04</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>52</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>11:10</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>105</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>11:12</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>60</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>11:19</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>86_EST CHICA-ESC AGRARIA</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>114</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>09:25:56</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
           <t>11:20</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
+      <c r="C151" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D141" t="n">
+      <c r="D151" t="n">
         <v>115</v>
       </c>
-      <c r="E141" t="inlineStr">
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>11:21</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>69</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>11:27</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>75</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>11:32</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>80</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>90</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>99</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>11:56</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>104</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>106</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>107</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>112</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>114</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>114</v>
+      </c>
+      <c r="E162" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -3895,7 +4420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3913,14 +4438,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:25:56</t>
+          <t>Última actualización: 10:12:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 18</t>
+          <t>Total filas: 20</t>
         </is>
       </c>
     </row>
@@ -4396,6 +4921,56 @@
         <v>96</v>
       </c>
       <c r="E23" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>11:02</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>99</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4412,7 +4987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4430,14 +5005,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 09:25:56</t>
+          <t>Última actualización: 10:12:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 30</t>
         </is>
       </c>
     </row>
@@ -5190,6 +5765,31 @@
       <c r="E34" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>112</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 381
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:12:35</t>
+          <t>Última actualización: 10:52:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 157</t>
+          <t>Total filas: 176</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,21 +3862,21 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>10:53</t>
+          <t>10:52</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3917,16 +3917,16 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>10:56</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,21 +3937,21 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:53</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -3962,21 +3962,21 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>11:02</t>
+          <t>10:54</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -3992,16 +3992,16 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>11:03</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,21 +4012,21 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>11:04</t>
+          <t>10:56</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4042,16 +4042,16 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>11:10</t>
+          <t>11:01</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4067,16 +4067,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>11:12</t>
+          <t>11:02</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4087,21 +4087,21 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:03</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4112,21 +4112,21 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>11:20</t>
+          <t>11:04</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4137,21 +4137,21 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:06</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4162,21 +4162,21 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:10</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4187,21 +4187,21 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:11</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4217,16 +4217,16 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:12</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4237,21 +4237,21 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4262,21 +4262,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>11:56</t>
+          <t>11:20</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4292,16 +4292,16 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,21 +4312,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4342,16 +4342,16 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4367,16 +4367,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4387,23 +4387,498 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>11:34</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>42</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>11:41</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>49</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
           <t>10:12:35</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>11:42</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>90</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>11:43</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>51</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>11:51</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>99</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>11:56</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>104</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>106</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>11:58</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>66</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>11:59</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>107</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>12:04</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>112</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
         <is>
           <t>12:06</t>
         </is>
       </c>
-      <c r="C162" t="inlineStr">
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>114</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>10:12:35</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>12:06</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D162" t="n">
+      <c r="D173" t="n">
         <v>114</v>
       </c>
-      <c r="E162" t="inlineStr">
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>12:09</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>77</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>86</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>88</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>89</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>92</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>104</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>106</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>116</v>
+      </c>
+      <c r="E181" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4420,7 +4895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4438,14 +4913,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:12:35</t>
+          <t>Última actualización: 10:52:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 20</t>
+          <t>Total filas: 21</t>
         </is>
       </c>
     </row>
@@ -4971,6 +5446,31 @@
         <v>99</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>88</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5005,7 +5505,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:12:35</t>
+          <t>Última actualización: 10:52:48</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 382
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:52:48</t>
+          <t>Última actualización: 11:17:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 176</t>
+          <t>Total filas: 194</t>
         </is>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -4237,12 +4237,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>11:19</t>
+          <t>11:17</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4251,7 +4251,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4262,21 +4262,21 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>11:20</t>
+          <t>11:17</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4287,21 +4287,21 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>11:21</t>
+          <t>11:18</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4312,21 +4312,21 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>11:26</t>
+          <t>11:19</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4337,21 +4337,21 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:20</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D160" t="n">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4367,16 +4367,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>11:32</t>
+          <t>11:21</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4392,16 +4392,16 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>11:34</t>
+          <t>11:26</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4412,21 +4412,21 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>11:41</t>
+          <t>11:27</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4442,16 +4442,16 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>11:42</t>
+          <t>11:32</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4467,16 +4467,16 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:34</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4487,21 +4487,21 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:35</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4512,21 +4512,21 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>11:56</t>
+          <t>11:41</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4542,16 +4542,16 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:42</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4567,16 +4567,16 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:43</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4592,16 +4592,16 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4617,16 +4617,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>11:56</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4667,16 +4667,16 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4687,21 +4687,21 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,21 +4712,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>12:18</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,21 +4737,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4762,21 +4762,21 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,21 +4787,21 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,21 +4812,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4837,21 +4837,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4867,18 +4867,468 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
+          <t>12:09</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>77</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>12:09</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>52</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>12:11</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>54</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>86</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>12:20</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>88</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>89</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>64</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>64</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>92</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>12:36</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>104</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>80</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>106</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>84</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
           <t>12:48</t>
         </is>
       </c>
-      <c r="C181" t="inlineStr">
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>91</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D181" t="n">
+      <c r="D195" t="n">
         <v>116</v>
       </c>
-      <c r="E181" t="inlineStr">
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>12:49</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>92</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>110</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>117</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>119</v>
+      </c>
+      <c r="E199" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -4895,7 +5345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4913,14 +5363,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:52:48</t>
+          <t>Última actualización: 11:17:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 21</t>
+          <t>Total filas: 23</t>
         </is>
       </c>
     </row>
@@ -5471,6 +5921,56 @@
         <v>88</v>
       </c>
       <c r="E26" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>12:21</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>64</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>117</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5487,7 +5987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5505,14 +6005,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 10:52:48</t>
+          <t>Última actualización: 11:17:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 30</t>
+          <t>Total filas: 31</t>
         </is>
       </c>
     </row>
@@ -6290,6 +6790,31 @@
       <c r="E35" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>12:54</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>97</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 383
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:17:08</t>
+          <t>Última actualización: 11:45:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 194</t>
+          <t>Total filas: 207</t>
         </is>
       </c>
     </row>
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -4587,21 +4587,21 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4612,21 +4612,21 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>11:56</t>
+          <t>11:46</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4637,21 +4637,21 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:47</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4667,16 +4667,16 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:51</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4692,16 +4692,16 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:56</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D174" t="n">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4712,21 +4712,21 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,21 +4737,21 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>11:58</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4767,16 +4767,16 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4792,16 +4792,16 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4817,16 +4817,16 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4837,21 +4837,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,12 +4862,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,21 +4887,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4917,16 +4917,16 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>12:11</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,12 +4937,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>12:18</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -4951,7 +4951,7 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4962,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:08</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4987,21 +4987,21 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,21 +5012,21 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5042,16 +5042,16 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:11</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5062,21 +5062,21 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5092,16 +5092,16 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:18</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,21 +5112,21 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5137,21 +5137,21 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5162,21 +5162,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5192,16 +5192,16 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5217,16 +5217,16 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:24</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5237,21 +5237,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>12:49</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5262,21 +5262,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,21 +5287,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5317,18 +5317,343 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>80</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>106</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>84</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>10:52:48</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>116</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>91</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>12:49</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>92</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>13:02</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>77</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>110</v>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>117</v>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
           <t>13:16</t>
         </is>
       </c>
-      <c r="C199" t="inlineStr">
+      <c r="C208" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D199" t="n">
+      <c r="D208" t="n">
         <v>119</v>
       </c>
-      <c r="E199" t="inlineStr">
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>92</v>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>95</v>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>96</v>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>102</v>
+      </c>
+      <c r="E212" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5363,7 +5688,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:17:08</t>
+          <t>Última actualización: 11:45:01</t>
         </is>
       </c>
     </row>
@@ -5987,7 +6312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6005,14 +6330,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:17:08</t>
+          <t>Última actualización: 11:45:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 31</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -6815,6 +7140,31 @@
       <c r="E36" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>106</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 384
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:01</t>
+          <t>Última actualización: 11:59:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 207</t>
+          <t>Total filas: 216</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1497,11 +1497,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4792,16 +4792,16 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>11:59</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4812,21 +4812,21 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>12:05</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4837,21 +4837,21 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:01</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4862,12 +4862,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:04</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4887,21 +4887,21 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:05</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D182" t="n">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4912,12 +4912,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -4926,7 +4926,7 @@
         </is>
       </c>
       <c r="D183" t="n">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4937,21 +4937,21 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>12:07</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,21 +4962,21 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>12:08</t>
+          <t>12:06</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4992,16 +4992,16 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,12 +5012,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5026,7 +5026,7 @@
         </is>
       </c>
       <c r="D187" t="n">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5042,16 +5042,16 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>12:11</t>
+          <t>12:07</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5067,16 +5067,16 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:08</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5087,21 +5087,21 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12:18</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5117,16 +5117,16 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>12:20</t>
+          <t>12:09</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5142,16 +5142,16 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:11</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D192" t="n">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5162,21 +5162,21 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,21 +5187,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>12:21</t>
+          <t>12:13</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5217,16 +5217,16 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>12:18</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5237,21 +5237,21 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:20</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5262,21 +5262,21 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,21 +5287,21 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,21 +5312,21 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:21</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5342,16 +5342,16 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:24</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5362,21 +5362,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5387,21 +5387,21 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5412,21 +5412,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5442,16 +5442,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>12:49</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5462,21 +5462,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5492,16 +5492,16 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5512,21 +5512,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5542,16 +5542,16 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,17 +5562,17 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D209" t="n">
@@ -5592,16 +5592,16 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5612,21 +5612,21 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,23 +5637,248 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>215D_EL PATO</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>117</v>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>11:17:08</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>119</v>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
           <t>11:45:01</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>92</v>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>95</v>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>96</v>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
         <is>
           <t>13:27</t>
         </is>
       </c>
-      <c r="C212" t="inlineStr">
+      <c r="C217" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D212" t="n">
+      <c r="D217" t="n">
         <v>102</v>
       </c>
-      <c r="E212" t="inlineStr">
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>92</v>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>112</v>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>117</v>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>118</v>
+      </c>
+      <c r="E221" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5670,7 +5895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5688,14 +5913,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:01</t>
+          <t>Última actualización: 11:59:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 23</t>
+          <t>Total filas: 24</t>
         </is>
       </c>
     </row>
@@ -6296,6 +6521,31 @@
         <v>117</v>
       </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>112</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6330,7 +6580,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:45:01</t>
+          <t>Última actualización: 11:59:06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 385
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E221"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:59:06</t>
+          <t>Última actualización: 12:27:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 216</t>
+          <t>Total filas: 228</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4712,7 +4712,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4722,11 +4722,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,7 +4737,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4747,11 +4747,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5087,7 +5087,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5097,11 +5097,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5122,11 +5122,11 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5362,21 +5362,21 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>12:35</t>
+          <t>12:27</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5412,21 +5412,21 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>12:36</t>
+          <t>12:35</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5437,12 +5437,12 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:36</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -5451,7 +5451,7 @@
         </is>
       </c>
       <c r="D204" t="n">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5462,21 +5462,21 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:37</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D205" t="n">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5487,21 +5487,21 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>12:41</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5512,21 +5512,21 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:41</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5537,21 +5537,21 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:47</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D208" t="n">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5562,12 +5562,12 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>12:49</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -5576,7 +5576,7 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,21 +5587,21 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:48</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5617,16 +5617,16 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>12:49</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5637,21 +5637,21 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>12:50</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5662,21 +5662,21 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5692,16 +5692,16 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5712,21 +5712,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5737,21 +5737,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,21 +5762,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5787,21 +5787,21 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5812,21 +5812,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5837,21 +5837,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,23 +5862,323 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D221" t="n">
+        <v>95</v>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>13:21</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D222" t="n">
+        <v>96</v>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D223" t="n">
+        <v>102</v>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
           <t>11:59:06</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>92</v>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>13:32</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>65</v>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>13:37</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>70</v>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>13:46</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>79</v>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>112</v>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>117</v>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
         <is>
           <t>13:57</t>
         </is>
       </c>
-      <c r="C221" t="inlineStr">
+      <c r="C230" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D221" t="n">
+      <c r="D230" t="n">
         <v>118</v>
       </c>
-      <c r="E221" t="inlineStr">
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>97</v>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>110</v>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>113</v>
+      </c>
+      <c r="E233" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -5895,7 +6195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5913,14 +6213,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:59:06</t>
+          <t>Última actualización: 12:27:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 24</t>
+          <t>Total filas: 25</t>
         </is>
       </c>
     </row>
@@ -6546,6 +6846,31 @@
         <v>112</v>
       </c>
       <c r="E29" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>113</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6562,7 +6887,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6580,14 +6905,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 11:59:06</t>
+          <t>Última actualización: 12:27:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -7413,6 +7738,31 @@
         <v>106</v>
       </c>
       <c r="E37" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14:09</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>102</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 386
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:27:08</t>
+          <t>Última actualización: 12:54:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 228</t>
+          <t>Total filas: 237</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4972,7 +4972,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5287,7 +5287,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5297,11 +5297,11 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,7 +5312,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5322,11 +5322,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5662,7 +5662,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5672,11 +5672,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,21 +5687,21 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5712,21 +5712,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>13:03</t>
+          <t>13:02</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5737,21 +5737,21 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>13:07</t>
+          <t>13:03</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D216" t="n">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5762,21 +5762,21 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>13:08</t>
+          <t>13:05</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5792,16 +5792,16 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>13:14</t>
+          <t>13:07</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>215D_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5812,21 +5812,21 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>13:16</t>
+          <t>13:08</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D219" t="n">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5837,21 +5837,21 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>13:17</t>
+          <t>13:14</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215D_EL PATO</t>
         </is>
       </c>
       <c r="D220" t="n">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5862,21 +5862,21 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D221" t="n">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5887,21 +5887,21 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:16</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D222" t="n">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5917,16 +5917,16 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:17</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -5937,21 +5937,21 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -5962,21 +5962,21 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:21</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -5987,21 +5987,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>13:37</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6012,21 +6012,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6042,16 +6042,16 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,21 +6062,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6087,21 +6087,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:35</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6117,16 +6117,16 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:37</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D231" t="n">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6142,16 +6142,16 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6162,23 +6162,248 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>13:47</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>53</v>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>57</v>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>112</v>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>117</v>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>11:59:06</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>118</v>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
           <t>12:27:08</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>97</v>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>110</v>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
         <is>
           <t>14:20</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C240" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D233" t="n">
+      <c r="D240" t="n">
         <v>113</v>
       </c>
-      <c r="E233" t="inlineStr">
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>87</v>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>105</v>
+      </c>
+      <c r="E242" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6213,7 +6438,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:27:08</t>
+          <t>Última actualización: 12:54:06</t>
         </is>
       </c>
     </row>
@@ -6887,7 +7112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6905,14 +7130,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:27:08</t>
+          <t>Última actualización: 12:54:06</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -7721,50 +7946,100 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>L6173</t>
+          <t>L6203</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>11:45:01</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>106</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>12:27:08</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>14:09</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D38" t="n">
+      <c r="D39" t="n">
         <v>102</v>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>119</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 387
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:06</t>
+          <t>Última actualización: 13:23:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 237</t>
+          <t>Total filas: 246</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2797,11 +2797,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4712,7 +4712,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4722,11 +4722,11 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D175" t="n">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4737,7 +4737,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4747,11 +4747,11 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D176" t="n">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5087,7 +5087,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5097,11 +5097,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5122,11 +5122,11 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5987,21 +5987,21 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>13:26</t>
+          <t>13:24</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6012,21 +6012,21 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>13:27</t>
+          <t>13:26</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6037,21 +6037,21 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>13:31</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6062,21 +6062,21 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>13:32</t>
+          <t>13:31</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6087,21 +6087,21 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>13:35</t>
+          <t>13:32</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D230" t="n">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6112,12 +6112,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>13:37</t>
+          <t>13:35</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -6126,7 +6126,7 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6137,21 +6137,21 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>13:46</t>
+          <t>13:36</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D232" t="n">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6162,21 +6162,21 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>13:47</t>
+          <t>13:37</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6187,21 +6187,21 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:46</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D234" t="n">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6212,21 +6212,21 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>13:51</t>
+          <t>13:47</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6237,21 +6237,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>13:56</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6267,16 +6267,16 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>13:57</t>
+          <t>13:51</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6287,21 +6287,21 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>13:56</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6312,21 +6312,21 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>13:57</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6342,16 +6342,16 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6362,21 +6362,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,23 +6387,248 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>110</v>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>113</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
           <t>12:54:06</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr">
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>87</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
         <is>
           <t>14:39</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr">
+      <c r="C245" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D242" t="n">
+      <c r="D245" t="n">
         <v>105</v>
       </c>
-      <c r="E242" t="inlineStr">
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>14:57</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>94</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>95</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>97</v>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>102</v>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>111</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>15:21</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>118</v>
+      </c>
+      <c r="E251" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6420,7 +6645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6438,14 +6663,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:06</t>
+          <t>Última actualización: 13:23:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 25</t>
+          <t>Total filas: 26</t>
         </is>
       </c>
     </row>
@@ -7096,6 +7321,31 @@
         <v>113</v>
       </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>95</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7130,7 +7380,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 12:54:06</t>
+          <t>Última actualización: 13:23:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 388
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:23:09</t>
+          <t>Última actualización: 14:00:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 246</t>
+          <t>Total filas: 268</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -6337,21 +6337,21 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>14:04</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6362,21 +6362,21 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>14:05</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6387,21 +6387,21 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>14:17</t>
+          <t>14:01</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6412,21 +6412,21 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,21 +6437,21 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>14:04</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6462,21 +6462,21 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>14:39</t>
+          <t>14:05</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D245" t="n">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6487,21 +6487,21 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>14:57</t>
+          <t>14:06</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D246" t="n">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6512,21 +6512,21 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:16</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D247" t="n">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6537,21 +6537,21 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:17</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D248" t="n">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6562,21 +6562,21 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D249" t="n">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6587,21 +6587,21 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>14:20</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,23 +6612,573 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>113</v>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>14:21</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>87</v>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>14:39</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>105</v>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>14:44</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>44</v>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>14:56</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>56</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
           <t>13:23:09</t>
         </is>
       </c>
-      <c r="B251" t="inlineStr">
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>14:57</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>94</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>14:58</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>95</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>97</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>15:04</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>64</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>15:05</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>102</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>15:10</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>70</v>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>15:13</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>73</v>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>15:14</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>111</v>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>80</v>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>13:23:09</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
         <is>
           <t>15:21</t>
         </is>
       </c>
-      <c r="C251" t="inlineStr">
+      <c r="C265" t="inlineStr">
         <is>
           <t>26_HERNANDEZ</t>
         </is>
       </c>
-      <c r="D251" t="n">
+      <c r="D265" t="n">
         <v>118</v>
       </c>
-      <c r="E251" t="inlineStr">
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>15:25</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>85</v>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>15:32</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>92</v>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>15:35</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>95</v>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>96</v>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>98</v>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>106</v>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>113</v>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>116</v>
+      </c>
+      <c r="E273" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -6645,7 +7195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6663,14 +7213,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:23:09</t>
+          <t>Última actualización: 14:00:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 26</t>
+          <t>Total filas: 28</t>
         </is>
       </c>
     </row>
@@ -7304,12 +7854,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>14:20</t>
+          <t>14:19</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -7318,7 +7868,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -7329,23 +7879,73 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>12:27:08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>113</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>13:23:09</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>14:58</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="D32" t="n">
         <v>95</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>98</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7362,7 +7962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7380,14 +7980,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 13:23:09</t>
+          <t>Última actualización: 14:00:52</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 37</t>
         </is>
       </c>
     </row>
@@ -8271,25 +8871,75 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>14:52</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>52</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>12:54:06</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B41" t="inlineStr">
         <is>
           <t>14:53</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>215D_LA PLATA</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="D41" t="n">
         <v>119</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>15:34</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>94</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 389
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E273"/>
+  <dimension ref="A1:E288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:00:52</t>
+          <t>Última actualización: 14:44:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 268</t>
+          <t>Total filas: 283</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5272,11 +5272,11 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,7 +5287,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5297,11 +5297,11 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -6412,7 +6412,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6422,11 +6422,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6712,21 +6712,21 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>14:56</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D255" t="n">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6737,12 +6737,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>14:57</t>
+          <t>14:56</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -6751,7 +6751,7 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6767,16 +6767,16 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>14:57</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6792,16 +6792,16 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6812,21 +6812,21 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6837,12 +6837,12 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -6851,7 +6851,7 @@
         </is>
       </c>
       <c r="D260" t="n">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6862,21 +6862,21 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,21 +6887,21 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,21 +6912,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6942,16 +6942,16 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6962,21 +6962,21 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6987,21 +6987,21 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D266" t="n">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7042,16 +7042,16 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7062,21 +7062,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7092,16 +7092,16 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7117,16 +7117,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7142,16 +7142,16 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7167,18 +7167,393 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>96</v>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>15:37</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>53</v>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>15:38</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>98</v>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>61</v>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>106</v>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>15:47</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>63</v>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>15:53</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>113</v>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
           <t>15:56</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>72</v>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>14:00:52</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>15:56</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D273" t="n">
+      <c r="D281" t="n">
         <v>116</v>
       </c>
-      <c r="E273" t="inlineStr">
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>77</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>16:02</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>78</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>91</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>96</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>97</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>118</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>119</v>
+      </c>
+      <c r="E288" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7195,7 +7570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7213,14 +7588,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:00:52</t>
+          <t>Última actualización: 14:44:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 28</t>
+          <t>Total filas: 29</t>
         </is>
       </c>
     </row>
@@ -7946,6 +8321,31 @@
         <v>98</v>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>96</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7962,7 +8362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7980,14 +8380,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:00:52</t>
+          <t>Última actualización: 14:44:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 37</t>
+          <t>Total filas: 39</t>
         </is>
       </c>
     </row>
@@ -8871,12 +9271,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>14:52</t>
+          <t>14:46</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -8885,7 +9285,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -8896,12 +9296,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:52</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -8910,7 +9310,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -8921,25 +9321,75 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>12:54:06</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>14:53</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>215D_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>119</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>14:00:52</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>15:34</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D43" t="n">
         <v>94</v>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>90</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 390
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E288"/>
+  <dimension ref="A1:E294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:25</t>
+          <t>Última actualización: 15:02:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 283</t>
+          <t>Total filas: 289</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4797,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5037,7 +5037,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5047,11 +5047,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -6837,21 +6837,21 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>15:04</t>
+          <t>15:03</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D260" t="n">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6887,12 +6887,12 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:04</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -6901,7 +6901,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6912,21 +6912,21 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>15:06</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D263" t="n">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -6937,21 +6937,21 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:06</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -6967,16 +6967,16 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>15:13</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -6987,12 +6987,12 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>15:14</t>
+          <t>15:13</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -7001,7 +7001,7 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7012,21 +7012,21 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>15:16</t>
+          <t>15:14</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D267" t="n">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7037,21 +7037,21 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>15:20</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D268" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7062,21 +7062,21 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>13:23:09</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>15:20</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D269" t="n">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7087,12 +7087,12 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>13:23:09</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>15:25</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -7101,7 +7101,7 @@
         </is>
       </c>
       <c r="D270" t="n">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7117,16 +7117,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:25</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7137,21 +7137,21 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>15:26</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7167,16 +7167,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:32</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7187,21 +7187,21 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:34</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7217,16 +7217,16 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:35</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7237,21 +7237,21 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>15:36</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7262,21 +7262,21 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>15:37</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D277" t="n">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7287,21 +7287,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>15:38</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D278" t="n">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7312,21 +7312,21 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D279" t="n">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7337,21 +7337,21 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:46</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D280" t="n">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7362,21 +7362,21 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:47</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7387,21 +7387,21 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7417,16 +7417,16 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D283" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,21 +7437,21 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7467,16 +7467,16 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7487,21 +7487,21 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7517,16 +7517,16 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7537,23 +7537,173 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
+          <t>15:02:32</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>16:08</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>66</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
           <t>14:44:25</t>
         </is>
       </c>
-      <c r="B288" t="inlineStr">
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>91</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>96</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>97</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>118</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
         <is>
           <t>16:43</t>
         </is>
       </c>
-      <c r="C288" t="inlineStr">
+      <c r="C293" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D288" t="n">
+      <c r="D293" t="n">
         <v>119</v>
       </c>
-      <c r="E288" t="inlineStr">
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>15:02:32</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>16:56</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>17_179 Y 38</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>114</v>
+      </c>
+      <c r="E294" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7588,7 +7738,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:25</t>
+          <t>Última actualización: 15:02:32</t>
         </is>
       </c>
     </row>
@@ -8362,7 +8512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8380,14 +8530,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 14:44:25</t>
+          <t>Última actualización: 15:02:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 39</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -9390,6 +9540,31 @@
       <c r="E44" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>15:02:32</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:53</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>111</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 391
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E294"/>
+  <dimension ref="A1:E315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:02:32</t>
+          <t>Última actualización: 15:51:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 289</t>
+          <t>Total filas: 310</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D186" t="n">
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5037,7 +5037,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -5047,11 +5047,11 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5272,11 +5272,11 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5312,7 +5312,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5322,11 +5322,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -7412,12 +7412,12 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -7426,7 +7426,7 @@
         </is>
       </c>
       <c r="D283" t="n">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,21 +7462,21 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7487,7 +7487,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7497,11 +7497,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7512,12 +7512,12 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -7526,7 +7526,7 @@
         </is>
       </c>
       <c r="D287" t="n">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7537,21 +7537,21 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7567,16 +7567,16 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7587,21 +7587,21 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7612,21 +7612,21 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D291" t="n">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7637,21 +7637,21 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:10</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D292" t="n">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7662,21 +7662,21 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="D293" t="n">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7687,23 +7687,548 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>225_C ROCA-H SUR</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>91</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>28</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>16:20</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>96</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>16:21</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>97</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>16:29</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>38</v>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>39</v>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>16:34</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>43</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>16:36</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>45</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>118</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>16:42</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>51</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>16:43</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>119</v>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>16:48</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>57</v>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>16:50</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>59</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
           <t>15:02:32</t>
         </is>
       </c>
-      <c r="B294" t="inlineStr">
+      <c r="B307" t="inlineStr">
         <is>
           <t>16:56</t>
         </is>
       </c>
-      <c r="C294" t="inlineStr">
+      <c r="C307" t="inlineStr">
         <is>
           <t>17_179 Y 38</t>
         </is>
       </c>
-      <c r="D294" t="n">
+      <c r="D307" t="n">
         <v>114</v>
       </c>
-      <c r="E294" t="inlineStr">
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>73</v>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>90</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>93</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>97</v>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>105</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>107</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>109</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>119</v>
+      </c>
+      <c r="E315" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -7720,7 +8245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7738,14 +8263,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:02:32</t>
+          <t>Última actualización: 15:51:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 29</t>
+          <t>Total filas: 32</t>
         </is>
       </c>
     </row>
@@ -8479,23 +9004,98 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16:19</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>28</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>14:44:25</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>16:20</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D35" t="n">
         <v>96</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>73</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>109</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8512,7 +9112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8530,14 +9130,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:02:32</t>
+          <t>Última actualización: 15:51:48</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -9521,12 +10121,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -9535,7 +10135,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -9546,23 +10146,98 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>14:44:25</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>16:14</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>90</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>16:52</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>61</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
           <t>15:02:32</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B47" t="inlineStr">
         <is>
           <t>16:53</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D47" t="n">
         <v>111</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>17:17</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>86</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 392
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E315"/>
+  <dimension ref="A1:E331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:51:48</t>
+          <t>Última actualización: 16:18:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 310</t>
+          <t>Total filas: 326</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1497,11 +1497,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3297,11 +3297,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4797,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4987,7 +4987,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4997,11 +4997,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5272,7 +5272,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5287,7 +5287,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5297,11 +5297,11 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5312,7 +5312,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5322,11 +5322,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5597,11 +5597,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,7 +6887,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6897,11 +6897,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -7862,21 +7862,21 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D301" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7887,21 +7887,21 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7917,16 +7917,16 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -7937,21 +7937,21 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:37</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D304" t="n">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -7962,21 +7962,21 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D305" t="n">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -7987,21 +7987,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8012,21 +8012,21 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,21 +8037,21 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8062,21 +8062,21 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8092,16 +8092,16 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -8126,7 +8126,7 @@
         </is>
       </c>
       <c r="D311" t="n">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8137,21 +8137,21 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D312" t="n">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8162,21 +8162,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8187,21 +8187,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8217,18 +8217,418 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>73</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>47</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>47</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>47</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>90</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>17:21</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>63</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>17:24</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>93</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>17:28</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>97</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>17:29</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>71</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>17:36</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>105</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>107</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>80</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>109</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
           <t>17:50</t>
         </is>
       </c>
-      <c r="C315" t="inlineStr">
+      <c r="C328" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D315" t="n">
+      <c r="D328" t="n">
         <v>119</v>
       </c>
-      <c r="E315" t="inlineStr">
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>93</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>94</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>106</v>
+      </c>
+      <c r="E331" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8245,7 +8645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8263,14 +8663,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:51:48</t>
+          <t>Última actualización: 16:18:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 32</t>
+          <t>Total filas: 33</t>
         </is>
       </c>
     </row>
@@ -9079,23 +9479,48 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17:05</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>47</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>15:51:48</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>17:40</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="D38" t="n">
         <v>109</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9112,7 +9537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9130,14 +9555,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 15:51:48</t>
+          <t>Última actualización: 16:18:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -10240,6 +10665,56 @@
       <c r="E48" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>17:20</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>62</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>106</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 393
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E331"/>
+  <dimension ref="A1:E340"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:00</t>
+          <t>Última actualización: 16:40:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 326</t>
+          <t>Total filas: 335</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
@@ -4937,7 +4937,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4947,11 +4947,11 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D184" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5087,7 +5087,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5097,11 +5097,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5122,11 +5122,11 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5162,7 +5162,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5172,11 +5172,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5197,11 +5197,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -6237,7 +6237,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -6247,11 +6247,11 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -6272,11 +6272,11 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7537,7 +7537,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,7 +7562,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7572,11 +7572,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7987,21 +7987,21 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:41</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8042,16 +8042,16 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8062,7 +8062,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,21 +8087,21 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8117,16 +8117,16 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D311" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8137,12 +8137,12 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -8151,7 +8151,7 @@
         </is>
       </c>
       <c r="D312" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8162,21 +8162,21 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D313" t="n">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8187,21 +8187,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8212,21 +8212,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8237,21 +8237,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8272,7 +8272,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D317" t="n">
@@ -8297,7 +8297,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D318" t="n">
@@ -8312,21 +8312,21 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,21 +8337,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,21 +8362,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8387,21 +8387,21 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8412,21 +8412,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8442,16 +8442,16 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8467,16 +8467,16 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8492,16 +8492,16 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,21 +8512,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8542,16 +8542,16 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8587,21 +8587,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8617,18 +8617,243 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
+          <t>17:38</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>80</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>109</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>61</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>119</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>93</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>94</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C331" t="inlineStr">
+      <c r="C337" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D331" t="n">
+      <c r="D337" t="n">
         <v>106</v>
       </c>
-      <c r="E331" t="inlineStr">
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>101</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>108</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>112</v>
+      </c>
+      <c r="E340" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8645,7 +8870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8663,14 +8888,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:00</t>
+          <t>Última actualización: 16:40:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 33</t>
+          <t>Total filas: 34</t>
         </is>
       </c>
     </row>
@@ -9521,6 +9746,31 @@
         <v>109</v>
       </c>
       <c r="E38" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>108</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9555,7 +9805,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:18:00</t>
+          <t>Última actualización: 16:40:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 394
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E340"/>
+  <dimension ref="A1:E352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:40:16</t>
+          <t>Última actualización: 16:52:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 335</t>
+          <t>Total filas: 347</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -6412,7 +6412,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6422,11 +6422,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7537,7 +7537,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,7 +7562,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7572,11 +7572,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -8062,7 +8062,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,7 +8087,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8097,11 +8097,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8187,21 +8187,21 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D314" t="n">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8212,21 +8212,21 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8237,21 +8237,21 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D316" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8262,21 +8262,21 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="D317" t="n">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8292,16 +8292,16 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8312,12 +8312,12 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -8326,7 +8326,7 @@
         </is>
       </c>
       <c r="D319" t="n">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,21 +8337,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8362,21 +8362,21 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8392,16 +8392,16 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D322" t="n">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8412,21 +8412,21 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:05</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D323" t="n">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8437,21 +8437,21 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D324" t="n">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8462,21 +8462,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,21 +8487,21 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D326" t="n">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8512,21 +8512,21 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,21 +8537,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8592,16 +8592,16 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,21 +8612,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,21 +8637,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8662,21 +8662,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:41</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8687,21 +8687,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>119</v>
+        <v>42</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8712,21 +8712,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8737,21 +8737,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8762,21 +8762,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,21 +8787,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8812,21 +8812,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8837,23 +8837,323 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>17:40</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>109</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
           <t>16:40:16</t>
         </is>
       </c>
-      <c r="B340" t="inlineStr">
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>17:41</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>61</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>17:45</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>53</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>15:51:48</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>119</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>17:51</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>93</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>17:52</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>94</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>106</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>101</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>92</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>95</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>108</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
         <is>
           <t>18:32</t>
         </is>
       </c>
-      <c r="C340" t="inlineStr">
+      <c r="C351" t="inlineStr">
         <is>
           <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D340" t="n">
+      <c r="D351" t="n">
         <v>112</v>
       </c>
-      <c r="E340" t="inlineStr">
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>116</v>
+      </c>
+      <c r="E352" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -8870,7 +9170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8888,14 +9188,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:40:16</t>
+          <t>Última actualización: 16:52:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 34</t>
+          <t>Total filas: 35</t>
         </is>
       </c>
     </row>
@@ -9754,23 +10054,48 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>95</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>16:40:16</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>18:28</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D39" t="n">
+      <c r="D40" t="n">
         <v>108</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9787,7 +10112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9805,14 +10130,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:40:16</t>
+          <t>Última actualización: 16:52:47</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -10946,23 +11271,48 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>71</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>16:18:00</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D51" t="n">
         <v>106</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 395
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E352"/>
+  <dimension ref="A1:E363"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:47</t>
+          <t>Última actualización: 17:15:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 347</t>
+          <t>Total filas: 358</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -4912,7 +4912,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4922,11 +4922,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,7 +6887,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6897,11 +6897,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,7 +7462,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -7472,11 +7472,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -8012,7 +8012,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8022,11 +8022,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,7 +8037,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8047,11 +8047,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8462,21 +8462,21 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8487,12 +8487,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -8501,7 +8501,7 @@
         </is>
       </c>
       <c r="D326" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8517,16 +8517,16 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,21 +8537,21 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8562,21 +8562,21 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:17</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8587,21 +8587,21 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8612,21 +8612,21 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,21 +8637,21 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>17:29</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8662,21 +8662,21 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8687,21 +8687,21 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8712,21 +8712,21 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>17:35</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D335" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8737,21 +8737,21 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:31</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D336" t="n">
-        <v>105</v>
+        <v>39</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8762,21 +8762,21 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,21 +8787,21 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8812,21 +8812,21 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8842,16 +8842,16 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8867,16 +8867,16 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>17:41</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8887,21 +8887,21 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8917,16 +8917,16 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -8937,21 +8937,21 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -8962,21 +8962,21 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:41</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -8987,21 +8987,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,21 +9012,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9037,21 +9037,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9062,21 +9062,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9087,21 +9087,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9112,21 +9112,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9137,23 +9137,298 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
+          <t>16:18:00</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>106</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>18:16</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>61</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>18:21</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>101</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
           <t>16:52:47</t>
         </is>
       </c>
-      <c r="B352" t="inlineStr">
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>18:24</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>92</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>70</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>95</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>108</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>112</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
         <is>
           <t>18:48</t>
         </is>
       </c>
-      <c r="C352" t="inlineStr">
+      <c r="C360" t="inlineStr">
         <is>
           <t>14X44_ABASTO</t>
         </is>
       </c>
-      <c r="D352" t="n">
+      <c r="D360" t="n">
         <v>116</v>
       </c>
-      <c r="E352" t="inlineStr">
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>104</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>110</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>116</v>
+      </c>
+      <c r="E363" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9170,7 +9445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9188,14 +9463,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:47</t>
+          <t>Última actualización: 17:15:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 35</t>
+          <t>Total filas: 36</t>
         </is>
       </c>
     </row>
@@ -10096,6 +10371,31 @@
         <v>108</v>
       </c>
       <c r="E40" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>104</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10112,7 +10412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10130,14 +10430,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 16:52:47</t>
+          <t>Última actualización: 17:15:09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 49</t>
         </is>
       </c>
     </row>
@@ -11246,12 +11546,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:18</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -11260,7 +11560,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -11271,50 +11571,125 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>18:03</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>71</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>16:18:00</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>18:04</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>106</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>97</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>109</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 396
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E363"/>
+  <dimension ref="A1:E379"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:09</t>
+          <t>Última actualización: 17:42:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 358</t>
+          <t>Total filas: 374</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2797,11 +2797,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -7487,7 +7487,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7497,11 +7497,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7522,11 +7522,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -8062,7 +8062,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,7 +8087,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8097,11 +8097,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D321" t="n">
@@ -8397,7 +8397,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D322" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D323" t="n">
@@ -8987,21 +8987,21 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9012,21 +9012,21 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>17:43</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9037,21 +9037,21 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>17:43</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9062,21 +9062,21 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D349" t="n">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>
@@ -9087,21 +9087,21 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
@@ -9112,21 +9112,21 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D351" t="n">
-        <v>45</v>
+        <v>119</v>
       </c>
       <c r="E351" t="inlineStr">
         <is>
@@ -9142,16 +9142,16 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D352" t="n">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E352" t="inlineStr">
         <is>
@@ -9162,21 +9162,21 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D353" t="n">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="E353" t="inlineStr">
         <is>
@@ -9187,21 +9187,21 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
@@ -9212,21 +9212,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9237,21 +9237,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9262,21 +9262,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9287,21 +9287,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9312,21 +9312,21 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9337,21 +9337,21 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9362,21 +9362,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9387,21 +9387,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9417,18 +9417,418 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
+          <t>18:25</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>70</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>18:27</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>95</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>108</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>18:32</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>112</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>18:35</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>53</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>16:52:47</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>18:48</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>116</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>18:54</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>72</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>74</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>104</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>110</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
           <t>19:11</t>
         </is>
       </c>
-      <c r="C363" t="inlineStr">
+      <c r="C373" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D363" t="n">
+      <c r="D373" t="n">
         <v>116</v>
       </c>
-      <c r="E363" t="inlineStr">
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D374" t="n">
+        <v>90</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D375" t="n">
+        <v>95</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D376" t="n">
+        <v>95</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D377" t="n">
+        <v>99</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D378" t="n">
+        <v>108</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>118</v>
+      </c>
+      <c r="E379" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9445,7 +9845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9463,14 +9863,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:09</t>
+          <t>Última actualización: 17:42:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 36</t>
+          <t>Total filas: 38</t>
         </is>
       </c>
     </row>
@@ -10329,21 +10729,21 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -10354,12 +10754,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -10368,7 +10768,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -10379,23 +10779,73 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>16:40:16</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>18:28</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>108</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>17:15:09</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>18:59</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="D42" t="n">
         <v>104</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>118</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10430,7 +10880,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:15:09</t>
+          <t>Última actualización: 17:42:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 397
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E379"/>
+  <dimension ref="A1:E400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:01</t>
+          <t>Última actualización: 17:57:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 374</t>
+          <t>Total filas: 395</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4797,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -5087,7 +5087,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5097,11 +5097,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5122,11 +5122,11 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -5662,7 +5662,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5672,11 +5672,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,7 +5687,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5697,11 +5697,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,7 +6887,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6897,11 +6897,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -7487,7 +7487,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7497,11 +7497,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7522,11 +7522,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D325" t="n">
@@ -8497,7 +8497,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -8762,7 +8762,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8772,11 +8772,11 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,7 +8787,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -8797,11 +8797,11 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -9022,7 +9022,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D347" t="n">
@@ -9047,7 +9047,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D348" t="n">
@@ -9212,21 +9212,21 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>17:57</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
@@ -9237,21 +9237,21 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>18:01</t>
+          <t>17:57</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D356" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E356" t="inlineStr">
         <is>
@@ -9262,21 +9262,21 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>17:57</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D357" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="E357" t="inlineStr">
         <is>
@@ -9287,21 +9287,21 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>17:58</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D358" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E358" t="inlineStr">
         <is>
@@ -9317,16 +9317,16 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D359" t="n">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E359" t="inlineStr">
         <is>
@@ -9342,16 +9342,16 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9362,21 +9362,21 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9387,21 +9387,21 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D362" t="n">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E362" t="inlineStr">
         <is>
@@ -9412,21 +9412,21 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D363" t="n">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="E363" t="inlineStr">
         <is>
@@ -9437,21 +9437,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D364" t="n">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="E364" t="inlineStr">
         <is>
@@ -9462,21 +9462,21 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,21 +9487,21 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9512,21 +9512,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9537,21 +9537,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9562,12 +9562,12 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>18:54</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
@@ -9576,7 +9576,7 @@
         </is>
       </c>
       <c r="D369" t="n">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9587,21 +9587,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9612,21 +9612,21 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9637,21 +9637,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9662,21 +9662,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9687,21 +9687,21 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9712,21 +9712,21 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9742,16 +9742,16 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9762,21 +9762,21 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9787,21 +9787,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9817,18 +9817,543 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
+          <t>18:54</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D379" t="n">
+        <v>72</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>18:55</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D380" t="n">
+        <v>58</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>18:56</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D381" t="n">
+        <v>74</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>18:58</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D382" t="n">
+        <v>61</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D383" t="n">
+        <v>104</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D384" t="n">
+        <v>67</v>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>19:05</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D385" t="n">
+        <v>110</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>19:11</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D386" t="n">
+        <v>116</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>19:12</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D387" t="n">
+        <v>90</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D388" t="n">
+        <v>79</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D389" t="n">
+        <v>95</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>19:17</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D390" t="n">
+        <v>95</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D391" t="n">
+        <v>83</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>19:20</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D392" t="n">
+        <v>83</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>19:21</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D393" t="n">
+        <v>99</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>19:29</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D394" t="n">
+        <v>92</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D395" t="n">
+        <v>108</v>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D396" t="n">
+        <v>94</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D397" t="n">
+        <v>102</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C379" t="inlineStr">
+      <c r="C398" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D379" t="n">
+      <c r="D398" t="n">
         <v>118</v>
       </c>
-      <c r="E379" t="inlineStr">
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>19:49</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D399" t="n">
+        <v>112</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>113</v>
+      </c>
+      <c r="E400" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -9845,7 +10370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9863,14 +10388,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:01</t>
+          <t>Última actualización: 17:57:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 38</t>
+          <t>Total filas: 40</t>
         </is>
       </c>
     </row>
@@ -10804,12 +11329,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -10818,7 +11343,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -10829,23 +11354,73 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>18:59</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>104</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>102</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>17:42:01</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D43" t="n">
+      <c r="D45" t="n">
         <v>118</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10862,7 +11437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10880,14 +11455,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:42:01</t>
+          <t>Última actualización: 17:57:54</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 49</t>
+          <t>Total filas: 51</t>
         </is>
       </c>
     </row>
@@ -12096,12 +12671,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -12110,7 +12685,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -12126,18 +12701,68 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>18:52</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>97</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>66</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>17:15:09</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>19:04</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
-      <c r="D54" t="n">
+      <c r="D56" t="n">
         <v>109</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 398
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E400"/>
+  <dimension ref="A1:E408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:54</t>
+          <t>Última actualización: 18:19:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 395</t>
+          <t>Total filas: 403</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3297,11 +3297,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3912,7 +3912,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3922,11 +3922,11 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -5162,7 +5162,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5172,11 +5172,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5197,11 +5197,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6412,7 +6412,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -6422,11 +6422,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6437,7 +6437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -6447,11 +6447,11 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D244" t="n">
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8012,7 +8012,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8022,11 +8022,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,7 +8037,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8047,11 +8047,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8612,7 +8612,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8622,11 +8622,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,7 +8637,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8647,11 +8647,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8887,7 +8887,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8897,11 +8897,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,7 +8912,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -8922,11 +8922,11 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -9222,7 +9222,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9247,7 +9247,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D356" t="n">
@@ -9512,21 +9512,21 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:19</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D367" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E367" t="inlineStr">
         <is>
@@ -9537,21 +9537,21 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9562,21 +9562,21 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -9587,21 +9587,21 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D370" t="n">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="E370" t="inlineStr">
         <is>
@@ -9617,16 +9617,16 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D371" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E371" t="inlineStr">
         <is>
@@ -9637,21 +9637,21 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>16:40:16</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D372" t="n">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="E372" t="inlineStr">
         <is>
@@ -9662,21 +9662,21 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D373" t="n">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="E373" t="inlineStr">
         <is>
@@ -9692,16 +9692,16 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D374" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E374" t="inlineStr">
         <is>
@@ -9717,16 +9717,16 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D375" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E375" t="inlineStr">
         <is>
@@ -9737,21 +9737,21 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>16:40:16</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D376" t="n">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E376" t="inlineStr">
         <is>
@@ -9767,16 +9767,16 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D377" t="n">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E377" t="inlineStr">
         <is>
@@ -9787,21 +9787,21 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D378" t="n">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="E378" t="inlineStr">
         <is>
@@ -9812,21 +9812,21 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>18:54</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D379" t="n">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9842,16 +9842,16 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>18:55</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9862,21 +9862,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9887,21 +9887,21 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:54</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9912,21 +9912,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9937,21 +9937,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9962,21 +9962,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9992,16 +9992,16 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10012,21 +10012,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10042,16 +10042,16 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10062,21 +10062,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10087,12 +10087,12 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -10101,7 +10101,7 @@
         </is>
       </c>
       <c r="D390" t="n">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10112,21 +10112,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10142,16 +10142,16 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10167,16 +10167,16 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10187,21 +10187,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10212,21 +10212,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10242,16 +10242,16 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10262,21 +10262,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10287,21 +10287,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10312,21 +10312,21 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10342,18 +10342,218 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
+          <t>19:31</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D400" t="n">
+        <v>94</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>19:39</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D401" t="n">
+        <v>102</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D402" t="n">
+        <v>118</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>19:49</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D403" t="n">
+        <v>112</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
           <t>19:50</t>
         </is>
       </c>
-      <c r="C400" t="inlineStr">
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D404" t="n">
+        <v>91</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
         <is>
           <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
-      <c r="D400" t="n">
+      <c r="D405" t="n">
         <v>113</v>
       </c>
-      <c r="E400" t="inlineStr">
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D406" t="n">
+        <v>95</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D407" t="n">
+        <v>100</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D408" t="n">
+        <v>111</v>
+      </c>
+      <c r="E408" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10388,7 +10588,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:54</t>
+          <t>Última actualización: 18:19:32</t>
         </is>
       </c>
     </row>
@@ -11437,7 +11637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11455,14 +11655,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 17:57:54</t>
+          <t>Última actualización: 18:19:32</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 51</t>
+          <t>Total filas: 52</t>
         </is>
       </c>
     </row>
@@ -12765,6 +12965,31 @@
       <c r="E56" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>95</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 399
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E408"/>
+  <dimension ref="A1:E419"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:19:32</t>
+          <t>Última actualización: 18:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 403</t>
+          <t>Total filas: 414</t>
         </is>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4987,7 +4987,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4997,11 +4997,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D197" t="n">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5597,11 +5597,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -6247,11 +6247,11 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -6272,11 +6272,11 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7537,7 +7537,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,7 +7562,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7572,11 +7572,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -8197,7 +8197,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D314" t="n">
@@ -8222,7 +8222,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D315" t="n">
@@ -8247,7 +8247,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D316" t="n">
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,7 +8537,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8547,11 +8547,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -9812,12 +9812,12 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:37</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -9826,7 +9826,7 @@
         </is>
       </c>
       <c r="D379" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E379" t="inlineStr">
         <is>
@@ -9837,21 +9837,21 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>18:38</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D380" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E380" t="inlineStr">
         <is>
@@ -9862,21 +9862,21 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D381" t="n">
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="E381" t="inlineStr">
         <is>
@@ -9887,21 +9887,21 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>18:54</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D382" t="n">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E382" t="inlineStr">
         <is>
@@ -9912,21 +9912,21 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>18:55</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D383" t="n">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="E383" t="inlineStr">
         <is>
@@ -9937,21 +9937,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9962,21 +9962,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9987,21 +9987,21 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:54</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D386" t="n">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10012,21 +10012,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10037,21 +10037,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10062,21 +10062,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10092,16 +10092,16 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10112,21 +10112,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10142,16 +10142,16 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10162,21 +10162,21 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10187,21 +10187,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10212,21 +10212,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10237,21 +10237,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10262,21 +10262,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10287,21 +10287,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10317,16 +10317,16 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10342,16 +10342,16 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10367,16 +10367,16 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10392,16 +10392,16 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10417,16 +10417,16 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10437,21 +10437,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -10476,7 +10476,7 @@
         </is>
       </c>
       <c r="D405" t="n">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10487,21 +10487,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10512,21 +10512,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10537,23 +10537,298 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
+          <t>17:42:01</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="D408" t="n">
+        <v>118</v>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>19:49</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D409" t="n">
+        <v>112</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
           <t>18:19:32</t>
         </is>
       </c>
-      <c r="B408" t="inlineStr">
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D410" t="n">
+        <v>91</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>17:57:54</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D411" t="n">
+        <v>113</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D412" t="n">
+        <v>95</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D413" t="n">
+        <v>100</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
         <is>
           <t>20:10</t>
         </is>
       </c>
-      <c r="C408" t="inlineStr">
+      <c r="C414" t="inlineStr">
         <is>
           <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
-      <c r="D408" t="n">
+      <c r="D414" t="n">
         <v>111</v>
       </c>
-      <c r="E408" t="inlineStr">
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D415" t="n">
+        <v>95</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D416" t="n">
+        <v>103</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D417" t="n">
+        <v>105</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D418" t="n">
+        <v>106</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>114</v>
+      </c>
+      <c r="E419" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10570,7 +10845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10588,14 +10863,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:19:32</t>
+          <t>Última actualización: 18:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 40</t>
+          <t>Total filas: 41</t>
         </is>
       </c>
     </row>
@@ -11621,6 +11896,31 @@
         <v>118</v>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>106</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11637,7 +11937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11655,14 +11955,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:19:32</t>
+          <t>Última actualización: 18:37:39</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 52</t>
+          <t>Total filas: 53</t>
         </is>
       </c>
     </row>
@@ -12971,23 +13271,48 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>76</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>18:19:32</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B58" t="inlineStr">
         <is>
           <t>19:54</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D57" t="n">
+      <c r="D58" t="n">
         <v>95</v>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 400
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E419"/>
+  <dimension ref="A1:E431"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:39</t>
+          <t>Última actualización: 18:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 414</t>
+          <t>Total filas: 426</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4797,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -5087,7 +5087,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -5097,11 +5097,11 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5112,7 +5112,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5122,11 +5122,11 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,7 +7462,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -7472,11 +7472,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D325" t="n">
@@ -8497,7 +8497,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -9462,7 +9462,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -9472,11 +9472,11 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9497,11 +9497,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -9937,21 +9937,21 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:49</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D384" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E384" t="inlineStr">
         <is>
@@ -9962,21 +9962,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:50</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D385" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E385" t="inlineStr">
         <is>
@@ -9987,12 +9987,12 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>18:54</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
@@ -10001,7 +10001,7 @@
         </is>
       </c>
       <c r="D386" t="n">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="E386" t="inlineStr">
         <is>
@@ -10012,21 +10012,21 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>18:55</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D387" t="n">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="E387" t="inlineStr">
         <is>
@@ -10037,21 +10037,21 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:53</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D388" t="n">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="E388" t="inlineStr">
         <is>
@@ -10062,21 +10062,21 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:54</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D389" t="n">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E389" t="inlineStr">
         <is>
@@ -10087,21 +10087,21 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D390" t="n">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="E390" t="inlineStr">
         <is>
@@ -10112,21 +10112,21 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D391" t="n">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E391" t="inlineStr">
         <is>
@@ -10142,16 +10142,16 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10167,16 +10167,16 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10187,12 +10187,12 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
@@ -10201,7 +10201,7 @@
         </is>
       </c>
       <c r="D394" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10212,21 +10212,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10237,21 +10237,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10262,21 +10262,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10287,12 +10287,12 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -10301,7 +10301,7 @@
         </is>
       </c>
       <c r="D398" t="n">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10317,16 +10317,16 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10337,21 +10337,21 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10367,16 +10367,16 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10392,16 +10392,16 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10412,21 +10412,21 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10437,21 +10437,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10467,16 +10467,16 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10487,21 +10487,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10512,21 +10512,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10537,21 +10537,21 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D408" t="n">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10567,16 +10567,16 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10587,21 +10587,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10617,7 +10617,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
@@ -10626,7 +10626,7 @@
         </is>
       </c>
       <c r="D411" t="n">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10637,21 +10637,21 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10662,21 +10662,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10687,21 +10687,21 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10712,21 +10712,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10737,21 +10737,21 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10762,21 +10762,21 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10787,21 +10787,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10812,23 +10812,323 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D419" t="n">
+        <v>62</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D420" t="n">
+        <v>62</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D421" t="n">
+        <v>95</v>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D422" t="n">
+        <v>100</v>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>18:19:32</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D423" t="n">
+        <v>111</v>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>20:11</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D424" t="n">
+        <v>82</v>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
           <t>18:37:39</t>
         </is>
       </c>
-      <c r="B419" t="inlineStr">
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D425" t="n">
+        <v>95</v>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D426" t="n">
+        <v>103</v>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D427" t="n">
+        <v>92</v>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>105</v>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>106</v>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>95</v>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
         <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C419" t="inlineStr">
+      <c r="C431" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D419" t="n">
+      <c r="D431" t="n">
         <v>114</v>
       </c>
-      <c r="E419" t="inlineStr">
+      <c r="E431" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -10845,7 +11145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10863,14 +11163,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:39</t>
+          <t>Última actualización: 18:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 41</t>
+          <t>Total filas: 42</t>
         </is>
       </c>
     </row>
@@ -11921,6 +12221,31 @@
         <v>106</v>
       </c>
       <c r="E46" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>95</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11937,7 +12262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11955,14 +12280,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:37:39</t>
+          <t>Última actualización: 18:49:07</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 53</t>
+          <t>Total filas: 55</t>
         </is>
       </c>
     </row>
@@ -13171,12 +13496,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>18:50</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -13185,7 +13510,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -13196,12 +13521,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -13210,7 +13535,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -13221,21 +13546,21 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -13246,12 +13571,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -13260,7 +13585,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -13271,50 +13596,100 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>76</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>18:19:32</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>19:54</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="D59" t="n">
         <v>95</v>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>110</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 401
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E431"/>
+  <dimension ref="A1:E435"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:49:07</t>
+          <t>Última actualización: 18:56:08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 426</t>
+          <t>Total filas: 430</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2787,7 +2787,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2797,11 +2797,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -5162,7 +5162,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5172,11 +5172,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5197,11 +5197,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -7487,7 +7487,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:02:32</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -7497,11 +7497,11 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D286" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7512,7 +7512,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>15:02:32</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -7522,11 +7522,11 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D287" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,7 +8537,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8547,11 +8547,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8887,7 +8887,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8897,11 +8897,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,7 +8912,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -8922,11 +8922,11 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -9337,7 +9337,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -9347,11 +9347,11 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D360" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E360" t="inlineStr">
         <is>
@@ -9362,7 +9362,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -9372,11 +9372,11 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D361" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E361" t="inlineStr">
         <is>
@@ -9537,7 +9537,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -9547,11 +9547,11 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9562,7 +9562,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -9572,11 +9572,11 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -10137,21 +10137,21 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D392" t="n">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E392" t="inlineStr">
         <is>
@@ -10162,21 +10162,21 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:57</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D393" t="n">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="E393" t="inlineStr">
         <is>
@@ -10187,21 +10187,21 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D394" t="n">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="E394" t="inlineStr">
         <is>
@@ -10212,21 +10212,21 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D395" t="n">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="E395" t="inlineStr">
         <is>
@@ -10237,21 +10237,21 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D396" t="n">
-        <v>110</v>
+        <v>4</v>
       </c>
       <c r="E396" t="inlineStr">
         <is>
@@ -10262,21 +10262,21 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10287,21 +10287,21 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10312,21 +10312,21 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10337,21 +10337,21 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10362,21 +10362,21 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D401" t="n">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="E401" t="inlineStr">
         <is>
@@ -10392,16 +10392,16 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D402" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E402" t="inlineStr">
         <is>
@@ -10412,21 +10412,21 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10437,21 +10437,21 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D404" t="n">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="E404" t="inlineStr">
         <is>
@@ -10462,21 +10462,21 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D405" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10492,16 +10492,16 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D406" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E406" t="inlineStr">
         <is>
@@ -10512,21 +10512,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10537,12 +10537,12 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -10551,7 +10551,7 @@
         </is>
       </c>
       <c r="D408" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10562,21 +10562,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10592,16 +10592,16 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10612,21 +10612,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10637,21 +10637,21 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10662,21 +10662,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10692,16 +10692,16 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10712,21 +10712,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10737,21 +10737,21 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10767,16 +10767,16 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10787,21 +10787,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10812,21 +10812,21 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10837,21 +10837,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10862,12 +10862,12 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
@@ -10876,7 +10876,7 @@
         </is>
       </c>
       <c r="D421" t="n">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10887,21 +10887,21 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10912,21 +10912,21 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10937,21 +10937,21 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10962,21 +10962,21 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10987,21 +10987,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11017,16 +11017,16 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D427" t="n">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11042,16 +11042,16 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D428" t="n">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11067,16 +11067,16 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11092,16 +11092,16 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11117,18 +11117,118 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>105</v>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>106</v>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>95</v>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
           <t>20:31</t>
         </is>
       </c>
-      <c r="C431" t="inlineStr">
+      <c r="C434" t="inlineStr">
         <is>
           <t>225_GOMEZ</t>
         </is>
       </c>
-      <c r="D431" t="n">
+      <c r="D434" t="n">
         <v>114</v>
       </c>
-      <c r="E431" t="inlineStr">
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>18:56:08</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>117</v>
+      </c>
+      <c r="E435" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11163,7 +11263,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:49:07</t>
+          <t>Última actualización: 18:56:08</t>
         </is>
       </c>
     </row>
@@ -12280,7 +12380,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:49:07</t>
+          <t>Última actualización: 18:56:08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 402
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E435"/>
+  <dimension ref="A1:E448"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:56:08</t>
+          <t>Última actualización: 19:15:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 430</t>
+          <t>Total filas: 443</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:14:19</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1472,11 +1472,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>06:14:19</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1497,11 +1497,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3887,7 +3887,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3897,11 +3897,11 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3937,7 +3937,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3947,11 +3947,11 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4912,7 +4912,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4922,11 +4922,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5272,11 +5272,11 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5287,7 +5287,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -5297,11 +5297,11 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D198" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D199" t="n">
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -8062,7 +8062,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,7 +8087,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8097,11 +8097,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
@@ -8397,7 +8397,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D322" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D323" t="n">
@@ -8762,7 +8762,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8772,11 +8772,11 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,7 +8787,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -8797,11 +8797,11 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -9462,7 +9462,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -9472,11 +9472,11 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9497,11 +9497,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -10147,7 +10147,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D392" t="n">
@@ -10172,7 +10172,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D393" t="n">
@@ -10412,21 +10412,21 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D403" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E403" t="inlineStr">
         <is>
@@ -10462,12 +10462,12 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -10476,7 +10476,7 @@
         </is>
       </c>
       <c r="D405" t="n">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E405" t="inlineStr">
         <is>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D406" t="n">
@@ -10512,21 +10512,21 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D407" t="n">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E407" t="inlineStr">
         <is>
@@ -10537,12 +10537,12 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -10551,7 +10551,7 @@
         </is>
       </c>
       <c r="D408" t="n">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="E408" t="inlineStr">
         <is>
@@ -10562,21 +10562,21 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10587,21 +10587,21 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D410" t="n">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E410" t="inlineStr">
         <is>
@@ -10612,21 +10612,21 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10637,21 +10637,21 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10662,21 +10662,21 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10687,21 +10687,21 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>19:31</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -10712,21 +10712,21 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D415" t="n">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="E415" t="inlineStr">
         <is>
@@ -10737,21 +10737,21 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10762,21 +10762,21 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -10787,21 +10787,21 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:31</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D418" t="n">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E418" t="inlineStr">
         <is>
@@ -10812,21 +10812,21 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D419" t="n">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="E419" t="inlineStr">
         <is>
@@ -10837,21 +10837,21 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D420" t="n">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="E420" t="inlineStr">
         <is>
@@ -10867,16 +10867,16 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D421" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E421" t="inlineStr">
         <is>
@@ -10887,21 +10887,21 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D422" t="n">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="E422" t="inlineStr">
         <is>
@@ -10912,21 +10912,21 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D423" t="n">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="E423" t="inlineStr">
         <is>
@@ -10937,21 +10937,21 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D424" t="n">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="E424" t="inlineStr">
         <is>
@@ -10967,16 +10967,16 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10987,21 +10987,21 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11017,16 +11017,16 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D427" t="n">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E427" t="inlineStr">
         <is>
@@ -11037,21 +11037,21 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D428" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E428" t="inlineStr">
         <is>
@@ -11062,21 +11062,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11087,21 +11087,21 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11112,21 +11112,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11137,21 +11137,21 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11167,16 +11167,16 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11187,21 +11187,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11212,23 +11212,348 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>95</v>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>20:12</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D436" t="n">
+        <v>57</v>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>103</v>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>92</v>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>105</v>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>106</v>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>18:49:07</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>20:24</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>95</v>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>18:37:39</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>114</v>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>20:44</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D443" t="n">
+        <v>89</v>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
           <t>18:56:08</t>
         </is>
       </c>
-      <c r="B435" t="inlineStr">
+      <c r="B444" t="inlineStr">
         <is>
           <t>20:53</t>
         </is>
       </c>
-      <c r="C435" t="inlineStr">
+      <c r="C444" t="inlineStr">
         <is>
           <t>11_ETCHEVERRY</t>
         </is>
       </c>
-      <c r="D435" t="n">
+      <c r="D444" t="n">
         <v>117</v>
       </c>
-      <c r="E435" t="inlineStr">
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>101</v>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>102</v>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>109</v>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>113</v>
+      </c>
+      <c r="E448" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11245,7 +11570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11263,14 +11588,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:56:08</t>
+          <t>Última actualización: 19:15:23</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 42</t>
+          <t>Total filas: 43</t>
         </is>
       </c>
     </row>
@@ -12346,6 +12671,31 @@
         <v>95</v>
       </c>
       <c r="E47" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>113</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12380,7 +12730,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 18:56:08</t>
+          <t>Última actualización: 19:15:23</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 403
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E448"/>
+  <dimension ref="A1:E458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:23</t>
+          <t>Última actualización: 19:39:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 443</t>
+          <t>Total filas: 453</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2562,7 +2562,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3287,7 +3287,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3297,11 +3297,11 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -4987,7 +4987,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4997,11 +4997,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -7537,7 +7537,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,7 +7562,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7572,11 +7572,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7887,7 +7887,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -7897,11 +7897,11 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D302" t="n">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7912,7 +7912,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -7922,11 +7922,11 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D303" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -8197,7 +8197,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D314" t="n">
@@ -8222,7 +8222,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D315" t="n">
@@ -8612,7 +8612,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -8622,11 +8622,11 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8637,7 +8637,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -8647,11 +8647,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -10737,7 +10737,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -10747,11 +10747,11 @@
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10762,7 +10762,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -10772,11 +10772,11 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -11112,21 +11112,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11137,21 +11137,21 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D432" t="n">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="E432" t="inlineStr">
         <is>
@@ -11162,21 +11162,21 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11187,21 +11187,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11212,21 +11212,21 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11242,16 +11242,16 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D436" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11262,21 +11262,21 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D437" t="n">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11287,21 +11287,21 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11312,21 +11312,21 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11342,16 +11342,16 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11367,16 +11367,16 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D441" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D442" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -11412,21 +11412,21 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11437,21 +11437,21 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:56:08</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11462,21 +11462,21 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11487,21 +11487,21 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11517,16 +11517,16 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11537,23 +11537,273 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>73</v>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>73</v>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>18:56:08</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>20:53</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D450" t="n">
+        <v>117</v>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
           <t>19:15:23</t>
         </is>
       </c>
-      <c r="B448" t="inlineStr">
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D451" t="n">
+        <v>101</v>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>77</v>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="D453" t="n">
+        <v>102</v>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>109</v>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
         <is>
           <t>21:08</t>
         </is>
       </c>
-      <c r="C448" t="inlineStr">
+      <c r="C455" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D448" t="n">
+      <c r="D455" t="n">
         <v>113</v>
       </c>
-      <c r="E448" t="inlineStr">
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D456" t="n">
+        <v>102</v>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D457" t="n">
+        <v>104</v>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>119</v>
+      </c>
+      <c r="E458" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11588,7 +11838,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:23</t>
+          <t>Última actualización: 19:39:27</t>
         </is>
       </c>
     </row>
@@ -12712,7 +12962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12730,14 +12980,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:15:23</t>
+          <t>Última actualización: 19:39:27</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 55</t>
+          <t>Total filas: 56</t>
         </is>
       </c>
     </row>
@@ -14140,6 +14390,31 @@
       <c r="E60" t="inlineStr">
         <is>
           <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>110</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>L6203</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 404
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E458"/>
+  <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:39:27</t>
+          <t>Última actualización: 19:52:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 453</t>
+          <t>Total filas: 461</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1887,7 +1887,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>06:43:12</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1897,11 +1897,11 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>06:43:12</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>07:45:49</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2972,11 +2972,11 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2987,7 +2987,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>07:45:49</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2997,11 +2997,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -5162,7 +5162,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5172,11 +5172,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5197,11 +5197,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -6247,11 +6247,11 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -6272,11 +6272,11 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8012,7 +8012,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8022,11 +8022,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,7 +8037,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8047,11 +8047,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D321" t="n">
@@ -8397,7 +8397,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D322" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D323" t="n">
@@ -8762,7 +8762,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8772,11 +8772,11 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,7 +8787,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -8797,11 +8797,11 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -9462,7 +9462,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -9472,11 +9472,11 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9497,11 +9497,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -10562,7 +10562,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -10572,11 +10572,11 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D410" t="n">
@@ -10612,7 +10612,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -10622,11 +10622,11 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -11062,21 +11062,21 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:52</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D429" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="E429" t="inlineStr">
         <is>
@@ -11092,16 +11092,16 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D430" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E430" t="inlineStr">
         <is>
@@ -11112,21 +11112,21 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D431" t="n">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E431" t="inlineStr">
         <is>
@@ -11147,7 +11147,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D432" t="n">
@@ -11162,21 +11162,21 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D433" t="n">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="E433" t="inlineStr">
         <is>
@@ -11187,21 +11187,21 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D434" t="n">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="E434" t="inlineStr">
         <is>
@@ -11212,7 +11212,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -11222,11 +11222,11 @@
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D435" t="n">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="E435" t="inlineStr">
         <is>
@@ -11237,12 +11237,12 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
@@ -11251,7 +11251,7 @@
         </is>
       </c>
       <c r="D436" t="n">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E436" t="inlineStr">
         <is>
@@ -11262,7 +11262,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -11272,11 +11272,11 @@
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D437" t="n">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="E437" t="inlineStr">
         <is>
@@ -11287,21 +11287,21 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D438" t="n">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E438" t="inlineStr">
         <is>
@@ -11312,7 +11312,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -11322,11 +11322,11 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11337,21 +11337,21 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>20:20</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11362,12 +11362,12 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:20</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
@@ -11376,7 +11376,7 @@
         </is>
       </c>
       <c r="D441" t="n">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E441" t="inlineStr">
         <is>
@@ -11387,21 +11387,21 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D442" t="n">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E442" t="inlineStr">
         <is>
@@ -11412,7 +11412,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -11422,11 +11422,11 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D443" t="n">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11437,21 +11437,21 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11462,12 +11462,12 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
@@ -11476,7 +11476,7 @@
         </is>
       </c>
       <c r="D445" t="n">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11487,21 +11487,21 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D446" t="n">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11512,21 +11512,21 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11537,21 +11537,21 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D448" t="n">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -11562,21 +11562,21 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D449" t="n">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -11587,21 +11587,21 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>18:56:08</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11612,21 +11612,21 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11637,21 +11637,21 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D452" t="n">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11667,16 +11667,16 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11687,21 +11687,21 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D454" t="n">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -11717,16 +11717,16 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D455" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -11737,21 +11737,21 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D456" t="n">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11762,21 +11762,21 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11787,23 +11787,223 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
+          <t>19:15:23</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>113</v>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>21:20</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D459" t="n">
+        <v>88</v>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
           <t>19:39:27</t>
         </is>
       </c>
-      <c r="B458" t="inlineStr">
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D460" t="n">
+        <v>102</v>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D461" t="n">
+        <v>90</v>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D462" t="n">
+        <v>104</v>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D463" t="n">
+        <v>105</v>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
         <is>
           <t>21:38</t>
         </is>
       </c>
-      <c r="C458" t="inlineStr">
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D464" t="n">
+        <v>106</v>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D458" t="n">
+      <c r="D465" t="n">
         <v>119</v>
       </c>
-      <c r="E458" t="inlineStr">
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D466" t="n">
+        <v>115</v>
+      </c>
+      <c r="E466" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -11820,7 +12020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11838,14 +12038,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:39:27</t>
+          <t>Última actualización: 19:52:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 43</t>
+          <t>Total filas: 45</t>
         </is>
       </c>
     </row>
@@ -12929,23 +13129,73 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>75</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>19:15:23</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>21:08</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D48" t="n">
+      <c r="D49" t="n">
         <v>113</v>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>115</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12962,7 +13212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12980,14 +13230,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:39:27</t>
+          <t>Última actualización: 19:52:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 56</t>
+          <t>Total filas: 57</t>
         </is>
       </c>
     </row>
@@ -14396,23 +14646,48 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>96</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>19:39:27</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="B62" t="inlineStr">
         <is>
           <t>21:29</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D61" t="n">
+      <c r="D62" t="n">
         <v>110</v>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>L6203</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 405
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E466"/>
+  <dimension ref="A1:E475"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:52:49</t>
+          <t>Última actualización: 20:12:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 461</t>
+          <t>Total filas: 470</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -7437,7 +7437,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -7447,11 +7447,11 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7462,7 +7462,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -7472,11 +7472,11 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -8512,7 +8512,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -8522,11 +8522,11 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8537,7 +8537,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -8547,11 +8547,11 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D328" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8887,7 +8887,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -8897,11 +8897,11 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8912,7 +8912,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -8922,11 +8922,11 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -9222,7 +9222,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9247,7 +9247,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D356" t="n">
@@ -10737,7 +10737,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -10747,11 +10747,11 @@
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D416" t="n">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="E416" t="inlineStr">
         <is>
@@ -10762,7 +10762,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -10772,11 +10772,11 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D417" t="n">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E417" t="inlineStr">
         <is>
@@ -11412,12 +11412,12 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
@@ -11426,7 +11426,7 @@
         </is>
       </c>
       <c r="D443" t="n">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="E443" t="inlineStr">
         <is>
@@ -11437,7 +11437,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11447,11 +11447,11 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11462,21 +11462,21 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11487,12 +11487,12 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
@@ -11501,7 +11501,7 @@
         </is>
       </c>
       <c r="D446" t="n">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E446" t="inlineStr">
         <is>
@@ -11512,21 +11512,21 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>20:30</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D447" t="n">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="E447" t="inlineStr">
         <is>
@@ -11537,12 +11537,12 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:30</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
@@ -11551,7 +11551,7 @@
         </is>
       </c>
       <c r="D448" t="n">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="E448" t="inlineStr">
         <is>
@@ -11562,21 +11562,21 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D449" t="n">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="E449" t="inlineStr">
         <is>
@@ -11587,21 +11587,21 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:34</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D450" t="n">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E450" t="inlineStr">
         <is>
@@ -11612,21 +11612,21 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>20:43</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D451" t="n">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="E451" t="inlineStr">
         <is>
@@ -11637,12 +11637,12 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>18:56:08</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
@@ -11651,7 +11651,7 @@
         </is>
       </c>
       <c r="D452" t="n">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E452" t="inlineStr">
         <is>
@@ -11662,21 +11662,21 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:46</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D453" t="n">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="E453" t="inlineStr">
         <is>
@@ -11692,16 +11692,16 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D454" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E454" t="inlineStr">
         <is>
@@ -11712,21 +11712,21 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D455" t="n">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="E455" t="inlineStr">
         <is>
@@ -11737,21 +11737,21 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D456" t="n">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11762,21 +11762,21 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11787,21 +11787,21 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11812,21 +11812,21 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11837,17 +11837,17 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D460" t="n">
@@ -11862,21 +11862,21 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D461" t="n">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11887,21 +11887,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11912,21 +11912,21 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D463" t="n">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11942,16 +11942,16 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D464" t="n">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11967,16 +11967,16 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11992,18 +11992,243 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D466" t="n">
+        <v>90</v>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D467" t="n">
+        <v>70</v>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>21:23</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D468" t="n">
+        <v>104</v>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D469" t="n">
+        <v>85</v>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D470" t="n">
+        <v>105</v>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D471" t="n">
+        <v>106</v>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D472" t="n">
+        <v>119</v>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D473" t="n">
+        <v>94</v>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C466" t="inlineStr">
+      <c r="C474" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D466" t="n">
+      <c r="D474" t="n">
         <v>115</v>
       </c>
-      <c r="E466" t="inlineStr">
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>22:07</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D475" t="n">
+        <v>115</v>
+      </c>
+      <c r="E475" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12020,7 +12245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12038,14 +12263,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:52:49</t>
+          <t>Última actualización: 20:12:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 45</t>
+          <t>Total filas: 46</t>
         </is>
       </c>
     </row>
@@ -13179,23 +13404,48 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>94</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>19:52:49</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D50" t="n">
+      <c r="D51" t="n">
         <v>115</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13212,7 +13462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13230,14 +13480,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 19:52:49</t>
+          <t>Última actualización: 20:12:55</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 57</t>
+          <t>Total filas: 59</t>
         </is>
       </c>
     </row>
@@ -14621,12 +14871,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:38</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -14635,7 +14885,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -14646,50 +14896,100 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>20:39</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>L6203</t>
+          <t>L6173</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>21:28</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>96</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
           <t>19:39:27</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>21:29</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D62" t="n">
+      <c r="D63" t="n">
         <v>110</v>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>L6203</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>22:04</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>112</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>L6173</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 406
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E475"/>
+  <dimension ref="A1:E484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:55</t>
+          <t>Última actualización: 20:34:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 470</t>
+          <t>Total filas: 479</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2287,7 +2287,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>07:58:19</t>
+          <t>06:57:11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>06:57:11</t>
+          <t>07:58:19</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2322,11 +2322,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3447,11 +3447,11 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3462,7 +3462,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3472,11 +3472,11 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -4912,7 +4912,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4922,11 +4922,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4962,7 +4962,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -5272,11 +5272,11 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D198" t="n">
@@ -5312,7 +5312,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -5322,11 +5322,11 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5662,7 +5662,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>12:54:06</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -5672,11 +5672,11 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5687,7 +5687,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>12:54:06</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -5697,11 +5697,11 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -9462,7 +9462,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -9472,11 +9472,11 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9497,11 +9497,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -10562,7 +10562,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -10572,11 +10572,11 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D410" t="n">
@@ -10612,7 +10612,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -10622,11 +10622,11 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10962,7 +10962,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -10972,11 +10972,11 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D425" t="n">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="E425" t="inlineStr">
         <is>
@@ -10987,7 +10987,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -10997,11 +10997,11 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D426" t="n">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E426" t="inlineStr">
         <is>
@@ -11312,7 +11312,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -11322,11 +11322,11 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D439" t="n">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="E439" t="inlineStr">
         <is>
@@ -11337,7 +11337,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -11347,11 +11347,11 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D440" t="n">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="E440" t="inlineStr">
         <is>
@@ -11697,7 +11697,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D454" t="n">
@@ -11722,7 +11722,7 @@
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D455" t="n">
@@ -11737,7 +11737,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>18:56:08</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -11747,11 +11747,11 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D456" t="n">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="E456" t="inlineStr">
         <is>
@@ -11762,21 +11762,21 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>18:56:08</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D457" t="n">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="E457" t="inlineStr">
         <is>
@@ -11787,21 +11787,21 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11812,7 +11812,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -11822,11 +11822,11 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11842,16 +11842,16 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11867,16 +11867,16 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D461" t="n">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11887,21 +11887,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11912,12 +11912,12 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
@@ -11926,7 +11926,7 @@
         </is>
       </c>
       <c r="D463" t="n">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11937,21 +11937,21 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D464" t="n">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11962,21 +11962,21 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:16</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11992,16 +11992,16 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12012,21 +12012,21 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12037,12 +12037,12 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
@@ -12051,7 +12051,7 @@
         </is>
       </c>
       <c r="D468" t="n">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12067,16 +12067,16 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D469" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -12087,21 +12087,21 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D470" t="n">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -12112,21 +12112,21 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D471" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12137,21 +12137,21 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D472" t="n">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12162,21 +12162,21 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D473" t="n">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12192,16 +12192,16 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12212,23 +12212,248 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
+          <t>19:39:27</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D475" t="n">
+        <v>119</v>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
           <t>20:12:55</t>
         </is>
       </c>
-      <c r="B475" t="inlineStr">
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>21:46</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D476" t="n">
+        <v>94</v>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>19:52:49</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D477" t="n">
+        <v>115</v>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>20:12:55</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
         <is>
           <t>22:07</t>
         </is>
       </c>
-      <c r="C475" t="inlineStr">
+      <c r="C478" t="inlineStr">
         <is>
           <t>17_ROMERO</t>
         </is>
       </c>
-      <c r="D475" t="n">
+      <c r="D478" t="n">
         <v>115</v>
       </c>
-      <c r="E475" t="inlineStr">
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D479" t="n">
+        <v>94</v>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D480" t="n">
+        <v>94</v>
+      </c>
+      <c r="E480" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>22:16</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D481" t="n">
+        <v>102</v>
+      </c>
+      <c r="E481" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D482" t="n">
+        <v>107</v>
+      </c>
+      <c r="E482" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D483" t="n">
+        <v>114</v>
+      </c>
+      <c r="E483" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D484" t="n">
+        <v>118</v>
+      </c>
+      <c r="E484" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12263,7 +12488,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:55</t>
+          <t>Última actualización: 20:34:16</t>
         </is>
       </c>
     </row>
@@ -13462,7 +13687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13480,14 +13705,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:12:55</t>
+          <t>Última actualización: 20:34:16</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 59</t>
+          <t>Total filas: 61</t>
         </is>
       </c>
     </row>
@@ -14988,6 +15213,56 @@
         <v>112</v>
       </c>
       <c r="E64" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>91</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>107</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 407
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E484"/>
+  <dimension ref="A1:E489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:16</t>
+          <t>Última actualización: 20:47:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 479</t>
+          <t>Total filas: 484</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4987,7 +4987,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4997,11 +4997,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -6862,7 +6862,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -6872,11 +6872,11 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D261" t="n">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6887,7 +6887,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -6897,11 +6897,11 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D262" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8012,7 +8012,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -8022,11 +8022,11 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8037,7 +8037,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -8047,11 +8047,11 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D321" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D323" t="n">
@@ -8762,7 +8762,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -8772,11 +8772,11 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D337" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8787,7 +8787,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -8797,11 +8797,11 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D338" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -9537,7 +9537,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -9547,11 +9547,11 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D368" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E368" t="inlineStr">
         <is>
@@ -9562,7 +9562,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -9572,11 +9572,11 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D369" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E369" t="inlineStr">
         <is>
@@ -10312,7 +10312,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -10322,11 +10322,11 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D399" t="n">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="E399" t="inlineStr">
         <is>
@@ -10337,7 +10337,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -10347,11 +10347,11 @@
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D400" t="n">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="E400" t="inlineStr">
         <is>
@@ -10647,7 +10647,7 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D412" t="n">
@@ -10662,7 +10662,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10672,11 +10672,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10687,7 +10687,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
@@ -10697,11 +10697,11 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D414" t="n">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E414" t="inlineStr">
         <is>
@@ -11437,7 +11437,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>18:37:39</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -11447,11 +11447,11 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D444" t="n">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="E444" t="inlineStr">
         <is>
@@ -11462,7 +11462,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>18:37:39</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -11472,11 +11472,11 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D445" t="n">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="E445" t="inlineStr">
         <is>
@@ -11812,7 +11812,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -11822,11 +11822,11 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11837,7 +11837,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -11847,11 +11847,11 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11887,21 +11887,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11912,21 +11912,21 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D463" t="n">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11937,12 +11937,12 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
@@ -11951,7 +11951,7 @@
         </is>
       </c>
       <c r="D464" t="n">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11962,21 +11962,21 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>21:16</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11987,21 +11987,21 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:16</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12012,12 +12012,12 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
@@ -12026,7 +12026,7 @@
         </is>
       </c>
       <c r="D467" t="n">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12037,21 +12037,21 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12062,7 +12062,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -12072,11 +12072,11 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D469" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -12087,12 +12087,12 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -12101,7 +12101,7 @@
         </is>
       </c>
       <c r="D470" t="n">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -12112,7 +12112,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -12122,11 +12122,11 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D471" t="n">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12137,21 +12137,21 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D472" t="n">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12162,7 +12162,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -12172,11 +12172,11 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D473" t="n">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12192,16 +12192,16 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12237,21 +12237,21 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D476" t="n">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -12262,12 +12262,12 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
@@ -12276,7 +12276,7 @@
         </is>
       </c>
       <c r="D477" t="n">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -12287,17 +12287,17 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D478" t="n">
@@ -12312,21 +12312,21 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D479" t="n">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12347,7 +12347,7 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D480" t="n">
@@ -12367,16 +12367,16 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>22:16</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D481" t="n">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12387,21 +12387,21 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D482" t="n">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12417,16 +12417,16 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:16</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D483" t="n">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12442,18 +12442,143 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D484" t="n">
+        <v>107</v>
+      </c>
+      <c r="E484" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>22:25</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D485" t="n">
+        <v>98</v>
+      </c>
+      <c r="E485" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D486" t="n">
+        <v>114</v>
+      </c>
+      <c r="E486" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
           <t>22:32</t>
         </is>
       </c>
-      <c r="C484" t="inlineStr">
+      <c r="C487" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
         </is>
       </c>
-      <c r="D484" t="n">
+      <c r="D487" t="n">
         <v>118</v>
       </c>
-      <c r="E484" t="inlineStr">
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D488" t="n">
+        <v>107</v>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D489" t="n">
+        <v>112</v>
+      </c>
+      <c r="E489" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12470,7 +12595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12488,14 +12613,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:16</t>
+          <t>Última actualización: 20:47:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 46</t>
+          <t>Total filas: 47</t>
         </is>
       </c>
     </row>
@@ -13671,6 +13796,31 @@
         <v>115</v>
       </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>112</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -13687,7 +13837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13705,14 +13855,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:34:16</t>
+          <t>Última actualización: 20:47:24</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 61</t>
+          <t>Total filas: 62</t>
         </is>
       </c>
     </row>
@@ -15246,23 +15396,48 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>93</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>20:34:16</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="B67" t="inlineStr">
         <is>
           <t>22:21</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
-      <c r="D66" t="n">
+      <c r="D67" t="n">
         <v>107</v>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 408
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E489"/>
+  <dimension ref="A1:E497"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:24</t>
+          <t>Última actualización: 20:54:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 484</t>
+          <t>Total filas: 492</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2337,7 +2337,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>07:19:37</t>
+          <t>08:19:33</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2347,11 +2347,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>08:19:33</t>
+          <t>07:19:37</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2372,11 +2372,11 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2747,11 +2747,11 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2762,7 +2762,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2772,11 +2772,11 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3847,11 +3847,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3862,7 +3862,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3872,11 +3872,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>86_EST CHICA-ESC AGRARIA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D156" t="n">
@@ -4272,7 +4272,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>86_EST CHICA-ESC AGRARIA</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -4912,7 +4912,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4922,11 +4922,11 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D183" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D184" t="n">
@@ -4962,7 +4962,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4972,11 +4972,11 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D185" t="n">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -4987,7 +4987,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4997,11 +4997,11 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D186" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -5022,11 +5022,11 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D187" t="n">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D188" t="n">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D202" t="n">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D203" t="n">
@@ -6587,7 +6587,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>12:27:08</t>
+          <t>14:00:52</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -6597,11 +6597,11 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D250" t="n">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6612,7 +6612,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>14:00:52</t>
+          <t>12:27:08</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -6622,11 +6622,11 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D251" t="n">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8062,7 +8062,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>16:18:00</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -8072,11 +8072,11 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8087,7 +8087,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>16:18:00</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -8097,11 +8097,11 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D310" t="n">
-        <v>119</v>
+        <v>25</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D325" t="n">
@@ -8497,7 +8497,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -9222,7 +9222,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D355" t="n">
@@ -9247,7 +9247,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D356" t="n">
@@ -9272,7 +9272,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D357" t="n">
@@ -11147,7 +11147,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D432" t="n">
@@ -11172,7 +11172,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D433" t="n">
@@ -11787,21 +11787,21 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D458" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="E458" t="inlineStr">
         <is>
@@ -11812,21 +11812,21 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D459" t="n">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="E459" t="inlineStr">
         <is>
@@ -11837,21 +11837,21 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:54</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D460" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E460" t="inlineStr">
         <is>
@@ -11862,21 +11862,21 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D461" t="n">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="E461" t="inlineStr">
         <is>
@@ -11887,21 +11887,21 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D462" t="n">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="E462" t="inlineStr">
         <is>
@@ -11912,21 +11912,21 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D463" t="n">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E463" t="inlineStr">
         <is>
@@ -11937,21 +11937,21 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D464" t="n">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="E464" t="inlineStr">
         <is>
@@ -11962,21 +11962,21 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:01</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D465" t="n">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="E465" t="inlineStr">
         <is>
@@ -11987,21 +11987,21 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>21:16</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D466" t="n">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="E466" t="inlineStr">
         <is>
@@ -12017,16 +12017,16 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D467" t="n">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E467" t="inlineStr">
         <is>
@@ -12037,21 +12037,21 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D468" t="n">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E468" t="inlineStr">
         <is>
@@ -12062,21 +12062,21 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:16</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D469" t="n">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="E469" t="inlineStr">
         <is>
@@ -12087,21 +12087,21 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>21:17</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D470" t="n">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="E470" t="inlineStr">
         <is>
@@ -12112,21 +12112,21 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D471" t="n">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="E471" t="inlineStr">
         <is>
@@ -12142,16 +12142,16 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D472" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E472" t="inlineStr">
         <is>
@@ -12162,21 +12162,21 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D473" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E473" t="inlineStr">
         <is>
@@ -12187,21 +12187,21 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D474" t="n">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E474" t="inlineStr">
         <is>
@@ -12212,21 +12212,21 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>19:39:27</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D475" t="n">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="E475" t="inlineStr">
         <is>
@@ -12237,21 +12237,21 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D476" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E476" t="inlineStr">
         <is>
@@ -12262,21 +12262,21 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D477" t="n">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="E477" t="inlineStr">
         <is>
@@ -12287,21 +12287,21 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>19:52:49</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D478" t="n">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="E478" t="inlineStr">
         <is>
@@ -12312,12 +12312,12 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
@@ -12326,7 +12326,7 @@
         </is>
       </c>
       <c r="D479" t="n">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E479" t="inlineStr">
         <is>
@@ -12337,21 +12337,21 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:39:27</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D480" t="n">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="E480" t="inlineStr">
         <is>
@@ -12362,21 +12362,21 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D481" t="n">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="E481" t="inlineStr">
         <is>
@@ -12387,21 +12387,21 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>22:15</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D482" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E482" t="inlineStr">
         <is>
@@ -12412,21 +12412,21 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>19:52:49</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>22:16</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D483" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E483" t="inlineStr">
         <is>
@@ -12437,21 +12437,21 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D484" t="n">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -12462,21 +12462,21 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>22:25</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D485" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12492,16 +12492,16 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D486" t="n">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="E486" t="inlineStr">
         <is>
@@ -12512,21 +12512,21 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D487" t="n">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -12537,21 +12537,21 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:16</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D488" t="n">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -12562,23 +12562,223 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
+          <t>20:54:01</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>22:18</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D489" t="n">
+        <v>84</v>
+      </c>
+      <c r="E489" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D490" t="n">
+        <v>107</v>
+      </c>
+      <c r="E490" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>20:54:01</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>22:24</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D491" t="n">
+        <v>90</v>
+      </c>
+      <c r="E491" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
           <t>20:47:24</t>
         </is>
       </c>
-      <c r="B489" t="inlineStr">
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>22:25</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D492" t="n">
+        <v>98</v>
+      </c>
+      <c r="E492" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D493" t="n">
+        <v>114</v>
+      </c>
+      <c r="E493" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D494" t="n">
+        <v>118</v>
+      </c>
+      <c r="E494" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D495" t="n">
+        <v>107</v>
+      </c>
+      <c r="E495" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
         <is>
           <t>22:39</t>
         </is>
       </c>
-      <c r="C489" t="inlineStr">
+      <c r="C496" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D489" t="n">
+      <c r="D496" t="n">
         <v>112</v>
       </c>
-      <c r="E489" t="inlineStr">
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>20:54:01</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>22:48</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D497" t="n">
+        <v>114</v>
+      </c>
+      <c r="E497" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12613,7 +12813,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:24</t>
+          <t>Última actualización: 20:54:01</t>
         </is>
       </c>
     </row>
@@ -13855,7 +14055,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:47:24</t>
+          <t>Última actualización: 20:54:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 409
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-15.xlsx
+++ b/data/horarios-141-2026-01-15.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E497"/>
+  <dimension ref="A1:E508"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:01</t>
+          <t>Última actualización: 22:01:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 492</t>
+          <t>Total filas: 503</t>
         </is>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>05:19:24</t>
+          <t>05:49:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1222,11 +1222,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>05:49:10</t>
+          <t>05:19:24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1247,11 +1247,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2787,7 +2787,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>08:48:09</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2797,11 +2797,11 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>08:48:09</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2822,11 +2822,11 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -3537,7 +3537,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>08:36:20</t>
+          <t>09:25:56</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3547,11 +3547,11 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>09:25:56</t>
+          <t>08:36:20</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3572,11 +3572,11 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3987,7 +3987,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3997,11 +3997,11 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4012,7 +4012,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -4022,11 +4022,11 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4762,7 +4762,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>10:12:35</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>10:12:35</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4797,11 +4797,11 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -5162,7 +5162,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>11:45:01</t>
+          <t>11:59:06</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -5172,11 +5172,11 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D193" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>11:59:06</t>
+          <t>11:45:01</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -5197,11 +5197,11 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5562,7 +5562,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>10:52:48</t>
+          <t>11:17:08</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -5572,11 +5572,11 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5587,7 +5587,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>11:17:08</t>
+          <t>10:52:48</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -5597,11 +5597,11 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -7537,7 +7537,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>14:44:25</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7562,7 +7562,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>14:44:25</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -7572,11 +7572,11 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D289" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -8312,7 +8312,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>15:51:48</t>
+          <t>16:52:47</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -8322,11 +8322,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8337,7 +8337,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>16:52:47</t>
+          <t>15:51:48</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D320" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -9462,7 +9462,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>17:15:09</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -9472,11 +9472,11 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D365" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E365" t="inlineStr">
         <is>
@@ -9487,7 +9487,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>17:15:09</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -9497,11 +9497,11 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D366" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E366" t="inlineStr">
         <is>
@@ -10262,7 +10262,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>18:19:32</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -10272,11 +10272,11 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D397" t="n">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E397" t="inlineStr">
         <is>
@@ -10287,7 +10287,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>18:19:32</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -10297,11 +10297,11 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D398" t="n">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E398" t="inlineStr">
         <is>
@@ -10562,7 +10562,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>17:57:54</t>
+          <t>19:15:23</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -10572,11 +10572,11 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D409" t="n">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="E409" t="inlineStr">
         <is>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D410" t="n">
@@ -10612,7 +10612,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>19:15:23</t>
+          <t>17:57:54</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -10622,11 +10622,11 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D411" t="n">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E411" t="inlineStr">
         <is>
@@ -10637,7 +10637,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>18:49:07</t>
+          <t>17:42:01</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -10647,11 +10647,11 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D412" t="n">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="E412" t="inlineStr">
         <is>
@@ -10662,7 +10662,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>17:42:01</t>
+          <t>18:49:07</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -10672,11 +10672,11 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D413" t="n">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="E413" t="inlineStr">
         <is>
@@ -10697,7 +10697,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D414" t="n">
@@ -11022,7 +11022,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D427" t="n">
@@ -11047,7 +11047,7 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D428" t="n">
@@ -12437,21 +12437,21 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>20:12:55</t>
+          <t>22:01:01</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>22:06</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D484" t="n">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E484" t="inlineStr">
         <is>
@@ -12462,12 +12462,12 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:12:55</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
@@ -12476,7 +12476,7 @@
         </is>
       </c>
       <c r="D485" t="n">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="E485" t="inlineStr">
         <is>
@@ -12497,7 +12497,7 @@
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D486" t="n">
@@ -12512,21 +12512,21 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>22:15</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D487" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E487" t="inlineStr">
         <is>
@@ -12537,12 +12537,12 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>22:16</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
@@ -12551,7 +12551,7 @@
         </is>
       </c>
       <c r="D488" t="n">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E488" t="inlineStr">
         <is>
@@ -12562,12 +12562,12 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>20:54:01</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>22:18</t>
+          <t>22:16</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
@@ -12576,7 +12576,7 @@
         </is>
       </c>
       <c r="D489" t="n">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="E489" t="inlineStr">
         <is>
@@ -12587,21 +12587,21 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:18</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D490" t="n">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E490" t="inlineStr">
         <is>
@@ -12612,21 +12612,21 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>20:54:01</t>
+          <t>22:01:01</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>22:24</t>
+          <t>22:21</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D491" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E491" t="inlineStr">
         <is>
@@ -12637,12 +12637,12 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>20:34:16</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>22:25</t>
+          <t>22:21</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
@@ -12651,7 +12651,7 @@
         </is>
       </c>
       <c r="D492" t="n">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E492" t="inlineStr">
         <is>
@@ -12662,21 +12662,21 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:54:01</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:24</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D493" t="n">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E493" t="inlineStr">
         <is>
@@ -12687,21 +12687,21 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>20:34:16</t>
+          <t>20:47:24</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>22:32</t>
+          <t>22:25</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D494" t="n">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="E494" t="inlineStr">
         <is>
@@ -12712,21 +12712,21 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>22:01:01</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>22:34</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D495" t="n">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="E495" t="inlineStr">
         <is>
@@ -12737,21 +12737,21 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>20:47:24</t>
+          <t>22:01:01</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D496" t="n">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="E496" t="inlineStr">
         <is>
@@ -12762,23 +12762,298 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>23_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D497" t="n">
+        <v>27</v>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D498" t="n">
+        <v>27</v>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>22:28</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="D499" t="n">
+        <v>114</v>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>20:34:16</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>22:32</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D500" t="n">
+        <v>118</v>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>22:34</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D501" t="n">
+        <v>107</v>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>20:47:24</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>22:39</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D502" t="n">
+        <v>112</v>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
           <t>20:54:01</t>
         </is>
       </c>
-      <c r="B497" t="inlineStr">
+      <c r="B503" t="inlineStr">
         <is>
           <t>22:48</t>
         </is>
       </c>
-      <c r="C497" t="inlineStr">
+      <c r="C503" t="inlineStr">
         <is>
           <t>14_ABASTO</t>
         </is>
       </c>
-      <c r="D497" t="n">
+      <c r="D503" t="n">
         <v>114</v>
       </c>
-      <c r="E497" t="inlineStr">
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>22:49</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="D504" t="n">
+        <v>48</v>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>14X44_ABASTO</t>
+        </is>
+      </c>
+      <c r="D505" t="n">
+        <v>67</v>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="D506" t="n">
+        <v>67</v>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>23:45</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D507" t="n">
+        <v>104</v>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>23:59</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D508" t="n">
+        <v>118</v>
+      </c>
+      <c r="E508" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -12795,7 +13070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12813,14 +13088,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:01</t>
+          <t>Última actualización: 22:01:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 47</t>
+          <t>Total filas: 48</t>
         </is>
       </c>
     </row>
@@ -14021,6 +14296,31 @@
         <v>112</v>
       </c>
       <c r="E52" t="inlineStr">
+        <is>
+          <t>LP1912</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>23:45</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>104</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>LP1912</t>
         </is>
@@ -14037,7 +14337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14055,14 +14355,14 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Última actualización: 20:54:01</t>
+          <t>Última actualización: 22:01:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Total filas: 62</t>
+          <t>Total filas: 64</t>
         </is>
       </c>
     </row>
@@ -15638,6 +15938,56 @@
         <v>107</v>
       </c>
       <c r="E67" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>26</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>L6173</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>22:01:01</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>67</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>L6173</t>
         </is>

</xml_diff>